<commit_message>
New update in test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/zltUI/ZltTestData.xlsx
+++ b/src/test/resources/testdata/zltUI/ZltTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gowthamraj\git\ZlaataQAseverNew\src\test\resources\testdata\zltUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B531FB-2864-44BB-9F6A-FFFC29A02664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B5ED01-420C-4C80-8914-7DD38238A4F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-Zlaata" sheetId="1" r:id="rId1"/>
     <sheet name="ZlaataTestData" sheetId="2" r:id="rId2"/>
+    <sheet name="ZlaataTestNewData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8389" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8497" uniqueCount="903">
   <si>
     <t>S.No</t>
   </si>
@@ -2732,6 +2733,9 @@
   </si>
   <si>
     <t>TD_UI_Zlaata_CP_21</t>
+  </si>
+  <si>
+    <t>ZlaataTestNewData</t>
   </si>
 </sst>
 </file>
@@ -3371,8 +3375,29 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3400,27 +3425,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4226,8 +4230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75D1F84-2AD1-4552-9C1F-85B59D75CCFA}">
   <dimension ref="A1:Z253"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" zoomScale="109" workbookViewId="0">
-      <selection activeCell="A180" sqref="A180:XFD180"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4980,18 +4984,18 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="94"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="94"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
-      <c r="J24" s="95"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="87"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
@@ -5378,18 +5382,18 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="96" t="s">
+      <c r="A37" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="97"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="97"/>
-      <c r="F37" s="97"/>
-      <c r="G37" s="97"/>
-      <c r="H37" s="97"/>
-      <c r="I37" s="97"/>
-      <c r="J37" s="98"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="89"/>
+      <c r="J37" s="90"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
@@ -5936,18 +5940,18 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="96" t="s">
+      <c r="A55" s="88" t="s">
         <v>244</v>
       </c>
-      <c r="B55" s="97"/>
-      <c r="C55" s="97"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="97"/>
-      <c r="F55" s="97"/>
-      <c r="G55" s="97"/>
-      <c r="H55" s="97"/>
-      <c r="I55" s="97"/>
-      <c r="J55" s="98"/>
+      <c r="B55" s="89"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="89"/>
+      <c r="E55" s="89"/>
+      <c r="F55" s="89"/>
+      <c r="G55" s="89"/>
+      <c r="H55" s="89"/>
+      <c r="I55" s="89"/>
+      <c r="J55" s="90"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="25">
@@ -6270,18 +6274,18 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="96" t="s">
+      <c r="A66" s="88" t="s">
         <v>246</v>
       </c>
-      <c r="B66" s="97"/>
-      <c r="C66" s="97"/>
-      <c r="D66" s="97"/>
-      <c r="E66" s="97"/>
-      <c r="F66" s="97"/>
-      <c r="G66" s="97"/>
-      <c r="H66" s="97"/>
-      <c r="I66" s="97"/>
-      <c r="J66" s="98"/>
+      <c r="B66" s="89"/>
+      <c r="C66" s="89"/>
+      <c r="D66" s="89"/>
+      <c r="E66" s="89"/>
+      <c r="F66" s="89"/>
+      <c r="G66" s="89"/>
+      <c r="H66" s="89"/>
+      <c r="I66" s="89"/>
+      <c r="J66" s="90"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="25">
@@ -6636,18 +6640,18 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="96" t="s">
+      <c r="A78" s="88" t="s">
         <v>345</v>
       </c>
-      <c r="B78" s="97"/>
-      <c r="C78" s="97"/>
-      <c r="D78" s="97"/>
-      <c r="E78" s="97"/>
-      <c r="F78" s="97"/>
-      <c r="G78" s="97"/>
-      <c r="H78" s="97"/>
-      <c r="I78" s="97"/>
-      <c r="J78" s="98"/>
+      <c r="B78" s="89"/>
+      <c r="C78" s="89"/>
+      <c r="D78" s="89"/>
+      <c r="E78" s="89"/>
+      <c r="F78" s="89"/>
+      <c r="G78" s="89"/>
+      <c r="H78" s="89"/>
+      <c r="I78" s="89"/>
+      <c r="J78" s="90"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="25">
@@ -7514,18 +7518,18 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="84" t="s">
+      <c r="A106" s="91" t="s">
         <v>374</v>
       </c>
-      <c r="B106" s="84"/>
-      <c r="C106" s="84"/>
-      <c r="D106" s="84"/>
-      <c r="E106" s="84"/>
-      <c r="F106" s="84"/>
-      <c r="G106" s="84"/>
-      <c r="H106" s="84"/>
-      <c r="I106" s="84"/>
-      <c r="J106" s="84"/>
+      <c r="B106" s="91"/>
+      <c r="C106" s="91"/>
+      <c r="D106" s="91"/>
+      <c r="E106" s="91"/>
+      <c r="F106" s="91"/>
+      <c r="G106" s="91"/>
+      <c r="H106" s="91"/>
+      <c r="I106" s="91"/>
+      <c r="J106" s="91"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="25">
@@ -8018,18 +8022,18 @@
       <c r="X120" s="58"/>
     </row>
     <row r="121" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="85" t="s">
+      <c r="A121" s="92" t="s">
         <v>376</v>
       </c>
-      <c r="B121" s="85"/>
-      <c r="C121" s="85"/>
-      <c r="D121" s="85"/>
-      <c r="E121" s="85"/>
-      <c r="F121" s="85"/>
-      <c r="G121" s="85"/>
-      <c r="H121" s="85"/>
-      <c r="I121" s="85"/>
-      <c r="J121" s="85"/>
+      <c r="B121" s="92"/>
+      <c r="C121" s="92"/>
+      <c r="D121" s="92"/>
+      <c r="E121" s="92"/>
+      <c r="F121" s="92"/>
+      <c r="G121" s="92"/>
+      <c r="H121" s="92"/>
+      <c r="I121" s="92"/>
+      <c r="J121" s="92"/>
       <c r="K121" s="57"/>
       <c r="L121" s="58"/>
       <c r="M121" s="58"/>
@@ -8092,18 +8096,18 @@
       <c r="X122" s="58"/>
     </row>
     <row r="123" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="85" t="s">
+      <c r="A123" s="92" t="s">
         <v>381</v>
       </c>
-      <c r="B123" s="85"/>
-      <c r="C123" s="85"/>
-      <c r="D123" s="85"/>
-      <c r="E123" s="85"/>
-      <c r="F123" s="85"/>
-      <c r="G123" s="85"/>
-      <c r="H123" s="85"/>
-      <c r="I123" s="85"/>
-      <c r="J123" s="85"/>
+      <c r="B123" s="92"/>
+      <c r="C123" s="92"/>
+      <c r="D123" s="92"/>
+      <c r="E123" s="92"/>
+      <c r="F123" s="92"/>
+      <c r="G123" s="92"/>
+      <c r="H123" s="92"/>
+      <c r="I123" s="92"/>
+      <c r="J123" s="92"/>
       <c r="K123" s="57"/>
       <c r="L123" s="58"/>
       <c r="M123" s="58"/>
@@ -8166,18 +8170,18 @@
       <c r="X124" s="58"/>
     </row>
     <row r="125" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="85" t="s">
+      <c r="A125" s="92" t="s">
         <v>394</v>
       </c>
-      <c r="B125" s="85"/>
-      <c r="C125" s="85"/>
-      <c r="D125" s="85"/>
-      <c r="E125" s="85"/>
-      <c r="F125" s="85"/>
-      <c r="G125" s="85"/>
-      <c r="H125" s="85"/>
-      <c r="I125" s="85"/>
-      <c r="J125" s="85"/>
+      <c r="B125" s="92"/>
+      <c r="C125" s="92"/>
+      <c r="D125" s="92"/>
+      <c r="E125" s="92"/>
+      <c r="F125" s="92"/>
+      <c r="G125" s="92"/>
+      <c r="H125" s="92"/>
+      <c r="I125" s="92"/>
+      <c r="J125" s="92"/>
     </row>
     <row r="126" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="25">
@@ -8502,18 +8506,18 @@
       <c r="X132" s="58"/>
     </row>
     <row r="133" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="85" t="s">
+      <c r="A133" s="92" t="s">
         <v>411</v>
       </c>
-      <c r="B133" s="85"/>
-      <c r="C133" s="85"/>
-      <c r="D133" s="86"/>
-      <c r="E133" s="86"/>
-      <c r="F133" s="86"/>
-      <c r="G133" s="86"/>
-      <c r="H133" s="86"/>
-      <c r="I133" s="86"/>
-      <c r="J133" s="86"/>
+      <c r="B133" s="92"/>
+      <c r="C133" s="92"/>
+      <c r="D133" s="93"/>
+      <c r="E133" s="93"/>
+      <c r="F133" s="93"/>
+      <c r="G133" s="93"/>
+      <c r="H133" s="93"/>
+      <c r="I133" s="93"/>
+      <c r="J133" s="93"/>
       <c r="K133" s="58"/>
       <c r="L133" s="58"/>
       <c r="M133" s="58"/>
@@ -9008,18 +9012,18 @@
       <c r="X144" s="58"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="90" t="s">
+      <c r="A145" s="97" t="s">
         <v>439</v>
       </c>
-      <c r="B145" s="91"/>
-      <c r="C145" s="91"/>
-      <c r="D145" s="91"/>
-      <c r="E145" s="91"/>
-      <c r="F145" s="91"/>
-      <c r="G145" s="91"/>
-      <c r="H145" s="91"/>
-      <c r="I145" s="91"/>
-      <c r="J145" s="92"/>
+      <c r="B145" s="98"/>
+      <c r="C145" s="98"/>
+      <c r="D145" s="98"/>
+      <c r="E145" s="98"/>
+      <c r="F145" s="98"/>
+      <c r="G145" s="98"/>
+      <c r="H145" s="98"/>
+      <c r="I145" s="98"/>
+      <c r="J145" s="99"/>
       <c r="K145" s="58"/>
       <c r="L145" s="58"/>
       <c r="M145" s="58"/>
@@ -9466,18 +9470,18 @@
       <c r="Z155" s="58"/>
     </row>
     <row r="156" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="85" t="s">
+      <c r="A156" s="92" t="s">
         <v>510</v>
       </c>
-      <c r="B156" s="85"/>
-      <c r="C156" s="85"/>
-      <c r="D156" s="85"/>
-      <c r="E156" s="85"/>
-      <c r="F156" s="85"/>
-      <c r="G156" s="85"/>
-      <c r="H156" s="85"/>
-      <c r="I156" s="85"/>
-      <c r="J156" s="85"/>
+      <c r="B156" s="92"/>
+      <c r="C156" s="92"/>
+      <c r="D156" s="92"/>
+      <c r="E156" s="92"/>
+      <c r="F156" s="92"/>
+      <c r="G156" s="92"/>
+      <c r="H156" s="92"/>
+      <c r="I156" s="92"/>
+      <c r="J156" s="92"/>
       <c r="K156" s="58"/>
       <c r="L156" s="58"/>
       <c r="M156" s="58"/>
@@ -9544,18 +9548,18 @@
       <c r="Z157" s="58"/>
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="85" t="s">
+      <c r="A158" s="92" t="s">
         <v>536</v>
       </c>
-      <c r="B158" s="85"/>
-      <c r="C158" s="85"/>
-      <c r="D158" s="85"/>
-      <c r="E158" s="85"/>
-      <c r="F158" s="85"/>
-      <c r="G158" s="85"/>
-      <c r="H158" s="85"/>
-      <c r="I158" s="85"/>
-      <c r="J158" s="85"/>
+      <c r="B158" s="92"/>
+      <c r="C158" s="92"/>
+      <c r="D158" s="92"/>
+      <c r="E158" s="92"/>
+      <c r="F158" s="92"/>
+      <c r="G158" s="92"/>
+      <c r="H158" s="92"/>
+      <c r="I158" s="92"/>
+      <c r="J158" s="92"/>
       <c r="K158" s="58"/>
       <c r="L158" s="58"/>
       <c r="M158" s="58"/>
@@ -10294,7 +10298,7 @@
       </c>
     </row>
     <row r="177" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="99">
+      <c r="A177" s="83">
         <v>19</v>
       </c>
       <c r="B177" s="69" t="s">
@@ -10307,7 +10311,7 @@
         <v>894</v>
       </c>
       <c r="E177" s="69" t="s">
-        <v>14</v>
+        <v>902</v>
       </c>
       <c r="F177" s="70" t="s">
         <v>895</v>
@@ -10326,7 +10330,7 @@
       </c>
     </row>
     <row r="178" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="99">
+      <c r="A178" s="83">
         <v>20</v>
       </c>
       <c r="B178" s="69" t="s">
@@ -10339,7 +10343,7 @@
         <v>897</v>
       </c>
       <c r="E178" s="69" t="s">
-        <v>14</v>
+        <v>902</v>
       </c>
       <c r="F178" s="70" t="s">
         <v>898</v>
@@ -10358,7 +10362,7 @@
       </c>
     </row>
     <row r="179" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="99">
+      <c r="A179" s="83">
         <v>21</v>
       </c>
       <c r="B179" s="69" t="s">
@@ -10371,7 +10375,7 @@
         <v>900</v>
       </c>
       <c r="E179" s="69" t="s">
-        <v>14</v>
+        <v>902</v>
       </c>
       <c r="F179" s="70" t="s">
         <v>901</v>
@@ -10390,18 +10394,18 @@
       </c>
     </row>
     <row r="180" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="85" t="s">
+      <c r="A180" s="92" t="s">
         <v>715</v>
       </c>
-      <c r="B180" s="85"/>
-      <c r="C180" s="85"/>
-      <c r="D180" s="83"/>
-      <c r="E180" s="85"/>
-      <c r="F180" s="85"/>
-      <c r="G180" s="85"/>
-      <c r="H180" s="85"/>
-      <c r="I180" s="85"/>
-      <c r="J180" s="85"/>
+      <c r="B180" s="92"/>
+      <c r="C180" s="92"/>
+      <c r="D180" s="84"/>
+      <c r="E180" s="92"/>
+      <c r="F180" s="92"/>
+      <c r="G180" s="92"/>
+      <c r="H180" s="92"/>
+      <c r="I180" s="92"/>
+      <c r="J180" s="92"/>
     </row>
     <row r="181" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="68">
@@ -10692,18 +10696,18 @@
       </c>
     </row>
     <row r="190" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="87" t="s">
+      <c r="A190" s="94" t="s">
         <v>617</v>
       </c>
-      <c r="B190" s="88"/>
-      <c r="C190" s="88"/>
-      <c r="D190" s="88"/>
-      <c r="E190" s="88"/>
-      <c r="F190" s="88"/>
-      <c r="G190" s="88"/>
-      <c r="H190" s="88"/>
-      <c r="I190" s="88"/>
-      <c r="J190" s="89"/>
+      <c r="B190" s="95"/>
+      <c r="C190" s="95"/>
+      <c r="D190" s="95"/>
+      <c r="E190" s="95"/>
+      <c r="F190" s="95"/>
+      <c r="G190" s="95"/>
+      <c r="H190" s="95"/>
+      <c r="I190" s="95"/>
+      <c r="J190" s="96"/>
     </row>
     <row r="191" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="68">
@@ -10930,18 +10934,18 @@
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A198" s="83" t="s">
+      <c r="A198" s="84" t="s">
         <v>638</v>
       </c>
-      <c r="B198" s="83"/>
-      <c r="C198" s="83"/>
-      <c r="D198" s="83"/>
-      <c r="E198" s="83"/>
-      <c r="F198" s="83"/>
-      <c r="G198" s="83"/>
-      <c r="H198" s="83"/>
-      <c r="I198" s="83"/>
-      <c r="J198" s="83"/>
+      <c r="B198" s="84"/>
+      <c r="C198" s="84"/>
+      <c r="D198" s="84"/>
+      <c r="E198" s="84"/>
+      <c r="F198" s="84"/>
+      <c r="G198" s="84"/>
+      <c r="H198" s="84"/>
+      <c r="I198" s="84"/>
+      <c r="J198" s="84"/>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="48">
@@ -11072,18 +11076,18 @@
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A203" s="83" t="s">
+      <c r="A203" s="84" t="s">
         <v>651</v>
       </c>
-      <c r="B203" s="83"/>
-      <c r="C203" s="83"/>
-      <c r="D203" s="83"/>
-      <c r="E203" s="83"/>
-      <c r="F203" s="83"/>
-      <c r="G203" s="83"/>
-      <c r="H203" s="83"/>
-      <c r="I203" s="83"/>
-      <c r="J203" s="83"/>
+      <c r="B203" s="84"/>
+      <c r="C203" s="84"/>
+      <c r="D203" s="84"/>
+      <c r="E203" s="84"/>
+      <c r="F203" s="84"/>
+      <c r="G203" s="84"/>
+      <c r="H203" s="84"/>
+      <c r="I203" s="84"/>
+      <c r="J203" s="84"/>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="48">
@@ -11118,18 +11122,18 @@
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A205" s="83" t="s">
+      <c r="A205" s="84" t="s">
         <v>657</v>
       </c>
-      <c r="B205" s="83"/>
-      <c r="C205" s="83"/>
-      <c r="D205" s="83"/>
-      <c r="E205" s="83"/>
-      <c r="F205" s="83"/>
-      <c r="G205" s="83"/>
-      <c r="H205" s="83"/>
-      <c r="I205" s="83"/>
-      <c r="J205" s="83"/>
+      <c r="B205" s="84"/>
+      <c r="C205" s="84"/>
+      <c r="D205" s="84"/>
+      <c r="E205" s="84"/>
+      <c r="F205" s="84"/>
+      <c r="G205" s="84"/>
+      <c r="H205" s="84"/>
+      <c r="I205" s="84"/>
+      <c r="J205" s="84"/>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="48">
@@ -11356,18 +11360,18 @@
       </c>
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A213" s="83" t="s">
+      <c r="A213" s="84" t="s">
         <v>733</v>
       </c>
-      <c r="B213" s="83"/>
-      <c r="C213" s="83"/>
-      <c r="D213" s="83"/>
-      <c r="E213" s="83"/>
-      <c r="F213" s="83"/>
-      <c r="G213" s="83"/>
-      <c r="H213" s="83"/>
-      <c r="I213" s="83"/>
-      <c r="J213" s="83"/>
+      <c r="B213" s="84"/>
+      <c r="C213" s="84"/>
+      <c r="D213" s="84"/>
+      <c r="E213" s="84"/>
+      <c r="F213" s="84"/>
+      <c r="G213" s="84"/>
+      <c r="H213" s="84"/>
+      <c r="I213" s="84"/>
+      <c r="J213" s="84"/>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="48">
@@ -11402,18 +11406,18 @@
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A215" s="83" t="s">
+      <c r="A215" s="84" t="s">
         <v>736</v>
       </c>
-      <c r="B215" s="83"/>
-      <c r="C215" s="83"/>
-      <c r="D215" s="83"/>
-      <c r="E215" s="83"/>
-      <c r="F215" s="83"/>
-      <c r="G215" s="83"/>
-      <c r="H215" s="83"/>
-      <c r="I215" s="83"/>
-      <c r="J215" s="83"/>
+      <c r="B215" s="84"/>
+      <c r="C215" s="84"/>
+      <c r="D215" s="84"/>
+      <c r="E215" s="84"/>
+      <c r="F215" s="84"/>
+      <c r="G215" s="84"/>
+      <c r="H215" s="84"/>
+      <c r="I215" s="84"/>
+      <c r="J215" s="84"/>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="48">
@@ -11512,18 +11516,18 @@
       </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A219" s="83" t="s">
+      <c r="A219" s="84" t="s">
         <v>746</v>
       </c>
-      <c r="B219" s="83"/>
-      <c r="C219" s="83"/>
-      <c r="D219" s="83"/>
-      <c r="E219" s="83"/>
-      <c r="F219" s="83"/>
-      <c r="G219" s="83"/>
-      <c r="H219" s="83"/>
-      <c r="I219" s="83"/>
-      <c r="J219" s="83"/>
+      <c r="B219" s="84"/>
+      <c r="C219" s="84"/>
+      <c r="D219" s="84"/>
+      <c r="E219" s="84"/>
+      <c r="F219" s="84"/>
+      <c r="G219" s="84"/>
+      <c r="H219" s="84"/>
+      <c r="I219" s="84"/>
+      <c r="J219" s="84"/>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="48">
@@ -11878,18 +11882,18 @@
       </c>
     </row>
     <row r="231" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="83" t="s">
+      <c r="A231" s="84" t="s">
         <v>783</v>
       </c>
-      <c r="B231" s="83"/>
-      <c r="C231" s="83"/>
-      <c r="D231" s="83"/>
-      <c r="E231" s="83"/>
-      <c r="F231" s="83"/>
-      <c r="G231" s="83"/>
-      <c r="H231" s="83"/>
-      <c r="I231" s="83"/>
-      <c r="J231" s="83"/>
+      <c r="B231" s="84"/>
+      <c r="C231" s="84"/>
+      <c r="D231" s="84"/>
+      <c r="E231" s="84"/>
+      <c r="F231" s="84"/>
+      <c r="G231" s="84"/>
+      <c r="H231" s="84"/>
+      <c r="I231" s="84"/>
+      <c r="J231" s="84"/>
     </row>
     <row r="232" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="48">
@@ -11924,18 +11928,18 @@
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A233" s="83" t="s">
+      <c r="A233" s="84" t="s">
         <v>796</v>
       </c>
-      <c r="B233" s="83"/>
-      <c r="C233" s="83"/>
-      <c r="D233" s="83"/>
-      <c r="E233" s="83"/>
-      <c r="F233" s="83"/>
-      <c r="G233" s="83"/>
-      <c r="H233" s="83"/>
-      <c r="I233" s="83"/>
-      <c r="J233" s="83"/>
+      <c r="B233" s="84"/>
+      <c r="C233" s="84"/>
+      <c r="D233" s="84"/>
+      <c r="E233" s="84"/>
+      <c r="F233" s="84"/>
+      <c r="G233" s="84"/>
+      <c r="H233" s="84"/>
+      <c r="I233" s="84"/>
+      <c r="J233" s="84"/>
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="48">
@@ -12322,18 +12326,18 @@
       </c>
     </row>
     <row r="246" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="83" t="s">
+      <c r="A246" s="84" t="s">
         <v>863</v>
       </c>
-      <c r="B246" s="83"/>
-      <c r="C246" s="83"/>
-      <c r="D246" s="83"/>
-      <c r="E246" s="83"/>
-      <c r="F246" s="83"/>
-      <c r="G246" s="83"/>
-      <c r="H246" s="83"/>
-      <c r="I246" s="83"/>
-      <c r="J246" s="83"/>
+      <c r="B246" s="84"/>
+      <c r="C246" s="84"/>
+      <c r="D246" s="84"/>
+      <c r="E246" s="84"/>
+      <c r="F246" s="84"/>
+      <c r="G246" s="84"/>
+      <c r="H246" s="84"/>
+      <c r="I246" s="84"/>
+      <c r="J246" s="84"/>
     </row>
     <row r="247" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="48">
@@ -12368,18 +12372,18 @@
       </c>
     </row>
     <row r="248" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="83" t="s">
+      <c r="A248" s="84" t="s">
         <v>866</v>
       </c>
-      <c r="B248" s="83"/>
-      <c r="C248" s="83"/>
-      <c r="D248" s="83"/>
-      <c r="E248" s="83"/>
-      <c r="F248" s="83"/>
-      <c r="G248" s="83"/>
-      <c r="H248" s="83"/>
-      <c r="I248" s="83"/>
-      <c r="J248" s="83"/>
+      <c r="B248" s="84"/>
+      <c r="C248" s="84"/>
+      <c r="D248" s="84"/>
+      <c r="E248" s="84"/>
+      <c r="F248" s="84"/>
+      <c r="G248" s="84"/>
+      <c r="H248" s="84"/>
+      <c r="I248" s="84"/>
+      <c r="J248" s="84"/>
     </row>
     <row r="249" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="48">
@@ -12543,15 +12547,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A215:J215"/>
-    <mergeCell ref="A213:J213"/>
-    <mergeCell ref="A205:J205"/>
-    <mergeCell ref="A219:J219"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="A55:J55"/>
-    <mergeCell ref="A66:J66"/>
-    <mergeCell ref="A78:J78"/>
     <mergeCell ref="A248:J248"/>
     <mergeCell ref="A106:J106"/>
     <mergeCell ref="A121:J121"/>
@@ -12568,6 +12563,15 @@
     <mergeCell ref="A158:J158"/>
     <mergeCell ref="A180:J180"/>
     <mergeCell ref="A231:J231"/>
+    <mergeCell ref="A215:J215"/>
+    <mergeCell ref="A213:J213"/>
+    <mergeCell ref="A205:J205"/>
+    <mergeCell ref="A219:J219"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A55:J55"/>
+    <mergeCell ref="A66:J66"/>
+    <mergeCell ref="A78:J78"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="E2:J2 E8:J21 E23:J23">
@@ -12667,8 +12671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE74813B-34A6-48F5-8B35-1C10409ED694}">
   <dimension ref="A1:AE237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A173" sqref="A173:XFD175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33069,4 +33073,366 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId50"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67D78B6-EF58-4C2E-A040-EC8FC2ED5646}">
+  <dimension ref="A1:AD4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>815</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>490</v>
+      </c>
+      <c r="V1" s="30" t="s">
+        <v>710</v>
+      </c>
+      <c r="W1" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="X1" s="30" t="s">
+        <v>711</v>
+      </c>
+      <c r="Y1" s="31" t="s">
+        <v>712</v>
+      </c>
+      <c r="Z1" s="31" t="s">
+        <v>713</v>
+      </c>
+      <c r="AA1" s="31" t="s">
+        <v>608</v>
+      </c>
+      <c r="AB1" s="31" t="s">
+        <v>602</v>
+      </c>
+      <c r="AC1" s="31" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD1" s="31" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="70" t="s">
+        <v>895</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+    </row>
+    <row r="3" spans="1:30" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70" t="s">
+        <v>898</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+    </row>
+    <row r="4" spans="1:30" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="70" t="s">
+        <v>901</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X4" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New  update in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/zltUI/ZltTestData.xlsx
+++ b/src/test/resources/testdata/zltUI/ZltTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gowthamraj\git\ZlaataQAseverNew\src\test\resources\testdata\zltUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B5ED01-420C-4C80-8914-7DD38238A4F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4324A-F31A-4C9C-A2B9-7A46A871C754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-Zlaata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8497" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8419" uniqueCount="903">
   <si>
     <t>S.No</t>
   </si>
@@ -3381,24 +3381,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3425,6 +3407,24 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4984,18 +4984,18 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="85" t="s">
+      <c r="A24" s="94" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="87"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="95"/>
+      <c r="J24" s="96"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
@@ -5382,18 +5382,18 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="88" t="s">
+      <c r="A37" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="89"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="89"/>
-      <c r="G37" s="89"/>
-      <c r="H37" s="89"/>
-      <c r="I37" s="89"/>
-      <c r="J37" s="90"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="98"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="98"/>
+      <c r="H37" s="98"/>
+      <c r="I37" s="98"/>
+      <c r="J37" s="99"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
@@ -5940,18 +5940,18 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="88" t="s">
+      <c r="A55" s="97" t="s">
         <v>244</v>
       </c>
-      <c r="B55" s="89"/>
-      <c r="C55" s="89"/>
-      <c r="D55" s="89"/>
-      <c r="E55" s="89"/>
-      <c r="F55" s="89"/>
-      <c r="G55" s="89"/>
-      <c r="H55" s="89"/>
-      <c r="I55" s="89"/>
-      <c r="J55" s="90"/>
+      <c r="B55" s="98"/>
+      <c r="C55" s="98"/>
+      <c r="D55" s="98"/>
+      <c r="E55" s="98"/>
+      <c r="F55" s="98"/>
+      <c r="G55" s="98"/>
+      <c r="H55" s="98"/>
+      <c r="I55" s="98"/>
+      <c r="J55" s="99"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="25">
@@ -6274,18 +6274,18 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="88" t="s">
+      <c r="A66" s="97" t="s">
         <v>246</v>
       </c>
-      <c r="B66" s="89"/>
-      <c r="C66" s="89"/>
-      <c r="D66" s="89"/>
-      <c r="E66" s="89"/>
-      <c r="F66" s="89"/>
-      <c r="G66" s="89"/>
-      <c r="H66" s="89"/>
-      <c r="I66" s="89"/>
-      <c r="J66" s="90"/>
+      <c r="B66" s="98"/>
+      <c r="C66" s="98"/>
+      <c r="D66" s="98"/>
+      <c r="E66" s="98"/>
+      <c r="F66" s="98"/>
+      <c r="G66" s="98"/>
+      <c r="H66" s="98"/>
+      <c r="I66" s="98"/>
+      <c r="J66" s="99"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="25">
@@ -6640,18 +6640,18 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="88" t="s">
+      <c r="A78" s="97" t="s">
         <v>345</v>
       </c>
-      <c r="B78" s="89"/>
-      <c r="C78" s="89"/>
-      <c r="D78" s="89"/>
-      <c r="E78" s="89"/>
-      <c r="F78" s="89"/>
-      <c r="G78" s="89"/>
-      <c r="H78" s="89"/>
-      <c r="I78" s="89"/>
-      <c r="J78" s="90"/>
+      <c r="B78" s="98"/>
+      <c r="C78" s="98"/>
+      <c r="D78" s="98"/>
+      <c r="E78" s="98"/>
+      <c r="F78" s="98"/>
+      <c r="G78" s="98"/>
+      <c r="H78" s="98"/>
+      <c r="I78" s="98"/>
+      <c r="J78" s="99"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="25">
@@ -7518,18 +7518,18 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="91" t="s">
+      <c r="A106" s="85" t="s">
         <v>374</v>
       </c>
-      <c r="B106" s="91"/>
-      <c r="C106" s="91"/>
-      <c r="D106" s="91"/>
-      <c r="E106" s="91"/>
-      <c r="F106" s="91"/>
-      <c r="G106" s="91"/>
-      <c r="H106" s="91"/>
-      <c r="I106" s="91"/>
-      <c r="J106" s="91"/>
+      <c r="B106" s="85"/>
+      <c r="C106" s="85"/>
+      <c r="D106" s="85"/>
+      <c r="E106" s="85"/>
+      <c r="F106" s="85"/>
+      <c r="G106" s="85"/>
+      <c r="H106" s="85"/>
+      <c r="I106" s="85"/>
+      <c r="J106" s="85"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="25">
@@ -8022,18 +8022,18 @@
       <c r="X120" s="58"/>
     </row>
     <row r="121" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="92" t="s">
+      <c r="A121" s="86" t="s">
         <v>376</v>
       </c>
-      <c r="B121" s="92"/>
-      <c r="C121" s="92"/>
-      <c r="D121" s="92"/>
-      <c r="E121" s="92"/>
-      <c r="F121" s="92"/>
-      <c r="G121" s="92"/>
-      <c r="H121" s="92"/>
-      <c r="I121" s="92"/>
-      <c r="J121" s="92"/>
+      <c r="B121" s="86"/>
+      <c r="C121" s="86"/>
+      <c r="D121" s="86"/>
+      <c r="E121" s="86"/>
+      <c r="F121" s="86"/>
+      <c r="G121" s="86"/>
+      <c r="H121" s="86"/>
+      <c r="I121" s="86"/>
+      <c r="J121" s="86"/>
       <c r="K121" s="57"/>
       <c r="L121" s="58"/>
       <c r="M121" s="58"/>
@@ -8096,18 +8096,18 @@
       <c r="X122" s="58"/>
     </row>
     <row r="123" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="92" t="s">
+      <c r="A123" s="86" t="s">
         <v>381</v>
       </c>
-      <c r="B123" s="92"/>
-      <c r="C123" s="92"/>
-      <c r="D123" s="92"/>
-      <c r="E123" s="92"/>
-      <c r="F123" s="92"/>
-      <c r="G123" s="92"/>
-      <c r="H123" s="92"/>
-      <c r="I123" s="92"/>
-      <c r="J123" s="92"/>
+      <c r="B123" s="86"/>
+      <c r="C123" s="86"/>
+      <c r="D123" s="86"/>
+      <c r="E123" s="86"/>
+      <c r="F123" s="86"/>
+      <c r="G123" s="86"/>
+      <c r="H123" s="86"/>
+      <c r="I123" s="86"/>
+      <c r="J123" s="86"/>
       <c r="K123" s="57"/>
       <c r="L123" s="58"/>
       <c r="M123" s="58"/>
@@ -8170,18 +8170,18 @@
       <c r="X124" s="58"/>
     </row>
     <row r="125" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="92" t="s">
+      <c r="A125" s="86" t="s">
         <v>394</v>
       </c>
-      <c r="B125" s="92"/>
-      <c r="C125" s="92"/>
-      <c r="D125" s="92"/>
-      <c r="E125" s="92"/>
-      <c r="F125" s="92"/>
-      <c r="G125" s="92"/>
-      <c r="H125" s="92"/>
-      <c r="I125" s="92"/>
-      <c r="J125" s="92"/>
+      <c r="B125" s="86"/>
+      <c r="C125" s="86"/>
+      <c r="D125" s="86"/>
+      <c r="E125" s="86"/>
+      <c r="F125" s="86"/>
+      <c r="G125" s="86"/>
+      <c r="H125" s="86"/>
+      <c r="I125" s="86"/>
+      <c r="J125" s="86"/>
     </row>
     <row r="126" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="25">
@@ -8506,18 +8506,18 @@
       <c r="X132" s="58"/>
     </row>
     <row r="133" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="92" t="s">
+      <c r="A133" s="86" t="s">
         <v>411</v>
       </c>
-      <c r="B133" s="92"/>
-      <c r="C133" s="92"/>
-      <c r="D133" s="93"/>
-      <c r="E133" s="93"/>
-      <c r="F133" s="93"/>
-      <c r="G133" s="93"/>
-      <c r="H133" s="93"/>
-      <c r="I133" s="93"/>
-      <c r="J133" s="93"/>
+      <c r="B133" s="86"/>
+      <c r="C133" s="86"/>
+      <c r="D133" s="87"/>
+      <c r="E133" s="87"/>
+      <c r="F133" s="87"/>
+      <c r="G133" s="87"/>
+      <c r="H133" s="87"/>
+      <c r="I133" s="87"/>
+      <c r="J133" s="87"/>
       <c r="K133" s="58"/>
       <c r="L133" s="58"/>
       <c r="M133" s="58"/>
@@ -9012,18 +9012,18 @@
       <c r="X144" s="58"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="97" t="s">
+      <c r="A145" s="91" t="s">
         <v>439</v>
       </c>
-      <c r="B145" s="98"/>
-      <c r="C145" s="98"/>
-      <c r="D145" s="98"/>
-      <c r="E145" s="98"/>
-      <c r="F145" s="98"/>
-      <c r="G145" s="98"/>
-      <c r="H145" s="98"/>
-      <c r="I145" s="98"/>
-      <c r="J145" s="99"/>
+      <c r="B145" s="92"/>
+      <c r="C145" s="92"/>
+      <c r="D145" s="92"/>
+      <c r="E145" s="92"/>
+      <c r="F145" s="92"/>
+      <c r="G145" s="92"/>
+      <c r="H145" s="92"/>
+      <c r="I145" s="92"/>
+      <c r="J145" s="93"/>
       <c r="K145" s="58"/>
       <c r="L145" s="58"/>
       <c r="M145" s="58"/>
@@ -9470,18 +9470,18 @@
       <c r="Z155" s="58"/>
     </row>
     <row r="156" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="92" t="s">
+      <c r="A156" s="86" t="s">
         <v>510</v>
       </c>
-      <c r="B156" s="92"/>
-      <c r="C156" s="92"/>
-      <c r="D156" s="92"/>
-      <c r="E156" s="92"/>
-      <c r="F156" s="92"/>
-      <c r="G156" s="92"/>
-      <c r="H156" s="92"/>
-      <c r="I156" s="92"/>
-      <c r="J156" s="92"/>
+      <c r="B156" s="86"/>
+      <c r="C156" s="86"/>
+      <c r="D156" s="86"/>
+      <c r="E156" s="86"/>
+      <c r="F156" s="86"/>
+      <c r="G156" s="86"/>
+      <c r="H156" s="86"/>
+      <c r="I156" s="86"/>
+      <c r="J156" s="86"/>
       <c r="K156" s="58"/>
       <c r="L156" s="58"/>
       <c r="M156" s="58"/>
@@ -9548,18 +9548,18 @@
       <c r="Z157" s="58"/>
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="92" t="s">
+      <c r="A158" s="86" t="s">
         <v>536</v>
       </c>
-      <c r="B158" s="92"/>
-      <c r="C158" s="92"/>
-      <c r="D158" s="92"/>
-      <c r="E158" s="92"/>
-      <c r="F158" s="92"/>
-      <c r="G158" s="92"/>
-      <c r="H158" s="92"/>
-      <c r="I158" s="92"/>
-      <c r="J158" s="92"/>
+      <c r="B158" s="86"/>
+      <c r="C158" s="86"/>
+      <c r="D158" s="86"/>
+      <c r="E158" s="86"/>
+      <c r="F158" s="86"/>
+      <c r="G158" s="86"/>
+      <c r="H158" s="86"/>
+      <c r="I158" s="86"/>
+      <c r="J158" s="86"/>
       <c r="K158" s="58"/>
       <c r="L158" s="58"/>
       <c r="M158" s="58"/>
@@ -10394,18 +10394,18 @@
       </c>
     </row>
     <row r="180" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="92" t="s">
+      <c r="A180" s="86" t="s">
         <v>715</v>
       </c>
-      <c r="B180" s="92"/>
-      <c r="C180" s="92"/>
+      <c r="B180" s="86"/>
+      <c r="C180" s="86"/>
       <c r="D180" s="84"/>
-      <c r="E180" s="92"/>
-      <c r="F180" s="92"/>
-      <c r="G180" s="92"/>
-      <c r="H180" s="92"/>
-      <c r="I180" s="92"/>
-      <c r="J180" s="92"/>
+      <c r="E180" s="86"/>
+      <c r="F180" s="86"/>
+      <c r="G180" s="86"/>
+      <c r="H180" s="86"/>
+      <c r="I180" s="86"/>
+      <c r="J180" s="86"/>
     </row>
     <row r="181" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="68">
@@ -10696,18 +10696,18 @@
       </c>
     </row>
     <row r="190" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="94" t="s">
+      <c r="A190" s="88" t="s">
         <v>617</v>
       </c>
-      <c r="B190" s="95"/>
-      <c r="C190" s="95"/>
-      <c r="D190" s="95"/>
-      <c r="E190" s="95"/>
-      <c r="F190" s="95"/>
-      <c r="G190" s="95"/>
-      <c r="H190" s="95"/>
-      <c r="I190" s="95"/>
-      <c r="J190" s="96"/>
+      <c r="B190" s="89"/>
+      <c r="C190" s="89"/>
+      <c r="D190" s="89"/>
+      <c r="E190" s="89"/>
+      <c r="F190" s="89"/>
+      <c r="G190" s="89"/>
+      <c r="H190" s="89"/>
+      <c r="I190" s="89"/>
+      <c r="J190" s="90"/>
     </row>
     <row r="191" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="68">
@@ -12547,6 +12547,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A215:J215"/>
+    <mergeCell ref="A213:J213"/>
+    <mergeCell ref="A205:J205"/>
+    <mergeCell ref="A219:J219"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A55:J55"/>
+    <mergeCell ref="A66:J66"/>
+    <mergeCell ref="A78:J78"/>
     <mergeCell ref="A248:J248"/>
     <mergeCell ref="A106:J106"/>
     <mergeCell ref="A121:J121"/>
@@ -12563,15 +12572,6 @@
     <mergeCell ref="A158:J158"/>
     <mergeCell ref="A180:J180"/>
     <mergeCell ref="A231:J231"/>
-    <mergeCell ref="A215:J215"/>
-    <mergeCell ref="A213:J213"/>
-    <mergeCell ref="A205:J205"/>
-    <mergeCell ref="A219:J219"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="A55:J55"/>
-    <mergeCell ref="A66:J66"/>
-    <mergeCell ref="A78:J78"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="E2:J2 E8:J21 E23:J23">
@@ -12669,10 +12669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE74813B-34A6-48F5-8B35-1C10409ED694}">
-  <dimension ref="A1:AE237"/>
+  <dimension ref="A1:AE234"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173:XFD175"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26945,9 +26945,9 @@
       <c r="AC172" s="28"/>
       <c r="AD172" s="28"/>
     </row>
-    <row r="173" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:30" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="70" t="s">
-        <v>895</v>
+        <v>601</v>
       </c>
       <c r="B173" s="48" t="s">
         <v>22</v>
@@ -27000,8 +27000,8 @@
       <c r="R173" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S173" s="48" t="s">
-        <v>22</v>
+      <c r="S173" s="49" t="s">
+        <v>841</v>
       </c>
       <c r="T173" s="48" t="s">
         <v>22</v>
@@ -27009,7 +27009,7 @@
       <c r="U173" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="V173" s="48" t="s">
+      <c r="V173" s="28" t="s">
         <v>22</v>
       </c>
       <c r="W173" s="28" t="s">
@@ -27024,14 +27024,22 @@
       <c r="Z173" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AA173" s="28"/>
-      <c r="AB173" s="28"/>
-      <c r="AC173" s="28"/>
-      <c r="AD173" s="28"/>
-    </row>
-    <row r="174" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA173" s="48" t="s">
+        <v>743</v>
+      </c>
+      <c r="AB173" s="36" t="s">
+        <v>603</v>
+      </c>
+      <c r="AC173" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD173" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="174" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="70" t="s">
-        <v>898</v>
+        <v>604</v>
       </c>
       <c r="B174" s="48" t="s">
         <v>22</v>
@@ -27084,8 +27092,8 @@
       <c r="R174" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S174" s="48" t="s">
-        <v>22</v>
+      <c r="S174" s="49" t="s">
+        <v>842</v>
       </c>
       <c r="T174" s="48" t="s">
         <v>22</v>
@@ -27093,7 +27101,7 @@
       <c r="U174" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="V174" s="48" t="s">
+      <c r="V174" s="28" t="s">
         <v>22</v>
       </c>
       <c r="W174" s="28" t="s">
@@ -27108,14 +27116,22 @@
       <c r="Z174" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AA174" s="28"/>
-      <c r="AB174" s="28"/>
-      <c r="AC174" s="28"/>
-      <c r="AD174" s="28"/>
-    </row>
-    <row r="175" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA174" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB174" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC174" s="73" t="s">
+        <v>836</v>
+      </c>
+      <c r="AD174" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="175" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="70" t="s">
-        <v>901</v>
+        <v>606</v>
       </c>
       <c r="B175" s="48" t="s">
         <v>22</v>
@@ -27168,8 +27184,8 @@
       <c r="R175" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S175" s="48" t="s">
-        <v>22</v>
+      <c r="S175" s="49" t="s">
+        <v>842</v>
       </c>
       <c r="T175" s="48" t="s">
         <v>22</v>
@@ -27177,7 +27193,7 @@
       <c r="U175" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="V175" s="48" t="s">
+      <c r="V175" s="28" t="s">
         <v>22</v>
       </c>
       <c r="W175" s="28" t="s">
@@ -27192,14 +27208,22 @@
       <c r="Z175" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AA175" s="28"/>
-      <c r="AB175" s="28"/>
-      <c r="AC175" s="28"/>
-      <c r="AD175" s="28"/>
-    </row>
-    <row r="176" spans="1:30" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA175" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB175" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC175" s="73" t="s">
+        <v>836</v>
+      </c>
+      <c r="AD175" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="176" spans="1:30" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="70" t="s">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="B176" s="48" t="s">
         <v>22</v>
@@ -27277,10 +27301,10 @@
         <v>22</v>
       </c>
       <c r="AA176" s="48" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="AB176" s="36" t="s">
-        <v>603</v>
+        <v>22</v>
       </c>
       <c r="AC176" s="48" t="s">
         <v>22</v>
@@ -27289,9 +27313,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="177" spans="1:31" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="70" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="B177" s="48" t="s">
         <v>22</v>
@@ -27374,8 +27398,8 @@
       <c r="AB177" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC177" s="73" t="s">
-        <v>836</v>
+      <c r="AC177" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD177" s="48" t="s">
         <v>22</v>
@@ -27383,7 +27407,7 @@
     </row>
     <row r="178" spans="1:31" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="70" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="B178" s="48" t="s">
         <v>22</v>
@@ -27473,9 +27497,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:31" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="70" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="B179" s="48" t="s">
         <v>22</v>
@@ -27529,7 +27553,7 @@
         <v>22</v>
       </c>
       <c r="S179" s="49" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="T179" s="48" t="s">
         <v>22</v>
@@ -27553,7 +27577,7 @@
         <v>22</v>
       </c>
       <c r="AA179" s="48" t="s">
-        <v>744</v>
+        <v>22</v>
       </c>
       <c r="AB179" s="36" t="s">
         <v>22</v>
@@ -27567,7 +27591,7 @@
     </row>
     <row r="180" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="70" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="B180" s="48" t="s">
         <v>22</v>
@@ -27621,7 +27645,7 @@
         <v>22</v>
       </c>
       <c r="S180" s="49" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="T180" s="48" t="s">
         <v>22</v>
@@ -27657,9 +27681,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="181" spans="1:31" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="70" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="B181" s="48" t="s">
         <v>22</v>
@@ -27713,7 +27737,7 @@
         <v>22</v>
       </c>
       <c r="S181" s="49" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="T181" s="48" t="s">
         <v>22</v>
@@ -27742,8 +27766,8 @@
       <c r="AB181" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC181" s="73" t="s">
-        <v>836</v>
+      <c r="AC181" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD181" s="48" t="s">
         <v>22</v>
@@ -27751,7 +27775,7 @@
     </row>
     <row r="182" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="70" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="B182" s="48" t="s">
         <v>22</v>
@@ -27805,7 +27829,7 @@
         <v>22</v>
       </c>
       <c r="S182" s="49" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="T182" s="48" t="s">
         <v>22</v>
@@ -27838,12 +27862,15 @@
         <v>22</v>
       </c>
       <c r="AD182" s="48" t="s">
-        <v>22</v>
+        <v>622</v>
+      </c>
+      <c r="AE182" s="80" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="183" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="70" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="B183" s="48" t="s">
         <v>22</v>
@@ -27897,7 +27924,7 @@
         <v>22</v>
       </c>
       <c r="S183" s="49" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="T183" s="48" t="s">
         <v>22</v>
@@ -27930,12 +27957,15 @@
         <v>22</v>
       </c>
       <c r="AD183" s="48" t="s">
-        <v>22</v>
+        <v>624</v>
+      </c>
+      <c r="AE183" s="80" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="184" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="70" t="s">
-        <v>614</v>
+        <v>629</v>
       </c>
       <c r="B184" s="48" t="s">
         <v>22</v>
@@ -27988,8 +28018,8 @@
       <c r="R184" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S184" s="49" t="s">
-        <v>845</v>
+      <c r="S184" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="T184" s="48" t="s">
         <v>22</v>
@@ -28022,12 +28052,15 @@
         <v>22</v>
       </c>
       <c r="AD184" s="48" t="s">
-        <v>22</v>
+        <v>641</v>
+      </c>
+      <c r="AE184" s="81" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="185" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="70" t="s">
-        <v>619</v>
+        <v>630</v>
       </c>
       <c r="B185" s="48" t="s">
         <v>22</v>
@@ -28080,8 +28113,8 @@
       <c r="R185" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S185" s="49" t="s">
-        <v>844</v>
+      <c r="S185" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="T185" s="48" t="s">
         <v>22</v>
@@ -28113,16 +28146,16 @@
       <c r="AC185" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AD185" s="48" t="s">
-        <v>622</v>
-      </c>
-      <c r="AE185" s="80" t="s">
-        <v>837</v>
+      <c r="AD185" s="77" t="s">
+        <v>633</v>
+      </c>
+      <c r="AE185" s="77" t="s">
+        <v>840</v>
       </c>
     </row>
     <row r="186" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="70" t="s">
-        <v>623</v>
+        <v>636</v>
       </c>
       <c r="B186" s="48" t="s">
         <v>22</v>
@@ -28175,8 +28208,8 @@
       <c r="R186" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S186" s="49" t="s">
-        <v>845</v>
+      <c r="S186" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="T186" s="48" t="s">
         <v>22</v>
@@ -28208,16 +28241,13 @@
       <c r="AC186" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AD186" s="48" t="s">
-        <v>624</v>
-      </c>
-      <c r="AE186" s="80" t="s">
-        <v>838</v>
+      <c r="AD186" s="77" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="187" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="70" t="s">
-        <v>629</v>
+        <v>878</v>
       </c>
       <c r="B187" s="48" t="s">
         <v>22</v>
@@ -28303,16 +28333,13 @@
       <c r="AC187" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AD187" s="48" t="s">
-        <v>641</v>
-      </c>
-      <c r="AE187" s="81" t="s">
-        <v>839</v>
+      <c r="AD187" s="77" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="188" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="70" t="s">
-        <v>630</v>
+        <v>879</v>
       </c>
       <c r="B188" s="48" t="s">
         <v>22</v>
@@ -28399,15 +28426,12 @@
         <v>22</v>
       </c>
       <c r="AD188" s="77" t="s">
-        <v>633</v>
-      </c>
-      <c r="AE188" s="77" t="s">
-        <v>840</v>
+        <v>884</v>
       </c>
     </row>
     <row r="189" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="70" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="B189" s="48" t="s">
         <v>22</v>
@@ -28493,13 +28517,13 @@
       <c r="AC189" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AD189" s="77" t="s">
-        <v>637</v>
+      <c r="AD189" s="48" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="190" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="70" t="s">
-        <v>878</v>
+        <v>642</v>
       </c>
       <c r="B190" s="48" t="s">
         <v>22</v>
@@ -28585,13 +28609,13 @@
       <c r="AC190" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AD190" s="77" t="s">
-        <v>880</v>
+      <c r="AD190" s="48" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="191" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="70" t="s">
-        <v>879</v>
+        <v>648</v>
       </c>
       <c r="B191" s="48" t="s">
         <v>22</v>
@@ -28677,13 +28701,13 @@
       <c r="AC191" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AD191" s="77" t="s">
-        <v>884</v>
+      <c r="AD191" s="48" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="192" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="70" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="B192" s="48" t="s">
         <v>22</v>
@@ -28775,7 +28799,7 @@
     </row>
     <row r="193" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="70" t="s">
-        <v>642</v>
+        <v>654</v>
       </c>
       <c r="B193" s="48" t="s">
         <v>22</v>
@@ -28828,8 +28852,8 @@
       <c r="R193" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S193" s="48" t="s">
-        <v>22</v>
+      <c r="S193" s="49" t="s">
+        <v>842</v>
       </c>
       <c r="T193" s="48" t="s">
         <v>22</v>
@@ -28858,8 +28882,8 @@
       <c r="AB193" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC193" s="48" t="s">
-        <v>22</v>
+      <c r="AC193" s="73" t="s">
+        <v>655</v>
       </c>
       <c r="AD193" s="48" t="s">
         <v>22</v>
@@ -28867,7 +28891,7 @@
     </row>
     <row r="194" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="70" t="s">
-        <v>648</v>
+        <v>656</v>
       </c>
       <c r="B194" s="48" t="s">
         <v>22</v>
@@ -28920,8 +28944,8 @@
       <c r="R194" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S194" s="48" t="s">
-        <v>22</v>
+      <c r="S194" s="49" t="s">
+        <v>844</v>
       </c>
       <c r="T194" s="48" t="s">
         <v>22</v>
@@ -28959,7 +28983,7 @@
     </row>
     <row r="195" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="70" t="s">
-        <v>649</v>
+        <v>662</v>
       </c>
       <c r="B195" s="48" t="s">
         <v>22</v>
@@ -29012,8 +29036,8 @@
       <c r="R195" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S195" s="48" t="s">
-        <v>22</v>
+      <c r="S195" s="49" t="s">
+        <v>845</v>
       </c>
       <c r="T195" s="48" t="s">
         <v>22</v>
@@ -29051,7 +29075,7 @@
     </row>
     <row r="196" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="70" t="s">
-        <v>654</v>
+        <v>665</v>
       </c>
       <c r="B196" s="48" t="s">
         <v>22</v>
@@ -29105,7 +29129,7 @@
         <v>22</v>
       </c>
       <c r="S196" s="49" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="T196" s="48" t="s">
         <v>22</v>
@@ -29134,8 +29158,8 @@
       <c r="AB196" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC196" s="73" t="s">
-        <v>655</v>
+      <c r="AC196" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD196" s="48" t="s">
         <v>22</v>
@@ -29143,7 +29167,7 @@
     </row>
     <row r="197" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="70" t="s">
-        <v>656</v>
+        <v>666</v>
       </c>
       <c r="B197" s="48" t="s">
         <v>22</v>
@@ -29197,7 +29221,7 @@
         <v>22</v>
       </c>
       <c r="S197" s="49" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="T197" s="48" t="s">
         <v>22</v>
@@ -29235,7 +29259,7 @@
     </row>
     <row r="198" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="70" t="s">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="B198" s="48" t="s">
         <v>22</v>
@@ -29289,7 +29313,7 @@
         <v>22</v>
       </c>
       <c r="S198" s="49" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="T198" s="48" t="s">
         <v>22</v>
@@ -29327,7 +29351,7 @@
     </row>
     <row r="199" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="70" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
       <c r="B199" s="48" t="s">
         <v>22</v>
@@ -29381,7 +29405,7 @@
         <v>22</v>
       </c>
       <c r="S199" s="49" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="T199" s="48" t="s">
         <v>22</v>
@@ -29419,7 +29443,7 @@
     </row>
     <row r="200" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="70" t="s">
-        <v>666</v>
+        <v>677</v>
       </c>
       <c r="B200" s="48" t="s">
         <v>22</v>
@@ -29473,7 +29497,7 @@
         <v>22</v>
       </c>
       <c r="S200" s="49" t="s">
-        <v>842</v>
+        <v>849</v>
       </c>
       <c r="T200" s="48" t="s">
         <v>22</v>
@@ -29511,7 +29535,7 @@
     </row>
     <row r="201" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="70" t="s">
-        <v>671</v>
+        <v>732</v>
       </c>
       <c r="B201" s="48" t="s">
         <v>22</v>
@@ -29565,7 +29589,7 @@
         <v>22</v>
       </c>
       <c r="S201" s="49" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="T201" s="48" t="s">
         <v>22</v>
@@ -29603,7 +29627,7 @@
     </row>
     <row r="202" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="70" t="s">
-        <v>676</v>
+        <v>738</v>
       </c>
       <c r="B202" s="48" t="s">
         <v>22</v>
@@ -29657,7 +29681,7 @@
         <v>22</v>
       </c>
       <c r="S202" s="49" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="T202" s="48" t="s">
         <v>22</v>
@@ -29695,7 +29719,7 @@
     </row>
     <row r="203" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="70" t="s">
-        <v>677</v>
+        <v>740</v>
       </c>
       <c r="B203" s="48" t="s">
         <v>22</v>
@@ -29749,7 +29773,7 @@
         <v>22</v>
       </c>
       <c r="S203" s="49" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="T203" s="48" t="s">
         <v>22</v>
@@ -29787,7 +29811,7 @@
     </row>
     <row r="204" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="70" t="s">
-        <v>732</v>
+        <v>780</v>
       </c>
       <c r="B204" s="48" t="s">
         <v>22</v>
@@ -29841,7 +29865,7 @@
         <v>22</v>
       </c>
       <c r="S204" s="49" t="s">
-        <v>842</v>
+        <v>850</v>
       </c>
       <c r="T204" s="48" t="s">
         <v>22</v>
@@ -29879,7 +29903,7 @@
     </row>
     <row r="205" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="70" t="s">
-        <v>738</v>
+        <v>745</v>
       </c>
       <c r="B205" s="48" t="s">
         <v>22</v>
@@ -29933,7 +29957,7 @@
         <v>22</v>
       </c>
       <c r="S205" s="49" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="T205" s="48" t="s">
         <v>22</v>
@@ -29971,7 +29995,7 @@
     </row>
     <row r="206" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="70" t="s">
-        <v>740</v>
+        <v>751</v>
       </c>
       <c r="B206" s="48" t="s">
         <v>22</v>
@@ -30025,7 +30049,7 @@
         <v>22</v>
       </c>
       <c r="S206" s="49" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="T206" s="48" t="s">
         <v>22</v>
@@ -30063,7 +30087,7 @@
     </row>
     <row r="207" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="70" t="s">
-        <v>780</v>
+        <v>752</v>
       </c>
       <c r="B207" s="48" t="s">
         <v>22</v>
@@ -30117,7 +30141,7 @@
         <v>22</v>
       </c>
       <c r="S207" s="49" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="T207" s="48" t="s">
         <v>22</v>
@@ -30155,7 +30179,7 @@
     </row>
     <row r="208" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="70" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="B208" s="48" t="s">
         <v>22</v>
@@ -30209,7 +30233,7 @@
         <v>22</v>
       </c>
       <c r="S208" s="49" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="T208" s="48" t="s">
         <v>22</v>
@@ -30247,7 +30271,7 @@
     </row>
     <row r="209" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="70" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="B209" s="48" t="s">
         <v>22</v>
@@ -30301,7 +30325,7 @@
         <v>22</v>
       </c>
       <c r="S209" s="49" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="T209" s="48" t="s">
         <v>22</v>
@@ -30339,7 +30363,7 @@
     </row>
     <row r="210" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="70" t="s">
-        <v>752</v>
+        <v>759</v>
       </c>
       <c r="B210" s="48" t="s">
         <v>22</v>
@@ -30393,7 +30417,7 @@
         <v>22</v>
       </c>
       <c r="S210" s="49" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="T210" s="48" t="s">
         <v>22</v>
@@ -30431,7 +30455,7 @@
     </row>
     <row r="211" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="70" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="B211" s="48" t="s">
         <v>22</v>
@@ -30485,7 +30509,7 @@
         <v>22</v>
       </c>
       <c r="S211" s="49" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="T211" s="48" t="s">
         <v>22</v>
@@ -30523,7 +30547,7 @@
     </row>
     <row r="212" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="70" t="s">
-        <v>758</v>
+        <v>767</v>
       </c>
       <c r="B212" s="48" t="s">
         <v>22</v>
@@ -30577,7 +30601,7 @@
         <v>22</v>
       </c>
       <c r="S212" s="49" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="T212" s="48" t="s">
         <v>22</v>
@@ -30615,7 +30639,7 @@
     </row>
     <row r="213" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="70" t="s">
-        <v>759</v>
+        <v>772</v>
       </c>
       <c r="B213" s="48" t="s">
         <v>22</v>
@@ -30669,7 +30693,7 @@
         <v>22</v>
       </c>
       <c r="S213" s="49" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="T213" s="48" t="s">
         <v>22</v>
@@ -30707,7 +30731,7 @@
     </row>
     <row r="214" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="70" t="s">
-        <v>764</v>
+        <v>775</v>
       </c>
       <c r="B214" s="48" t="s">
         <v>22</v>
@@ -30761,7 +30785,7 @@
         <v>22</v>
       </c>
       <c r="S214" s="49" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="T214" s="48" t="s">
         <v>22</v>
@@ -30799,7 +30823,7 @@
     </row>
     <row r="215" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="70" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
       <c r="B215" s="48" t="s">
         <v>22</v>
@@ -30853,7 +30877,7 @@
         <v>22</v>
       </c>
       <c r="S215" s="49" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="T215" s="48" t="s">
         <v>22</v>
@@ -30891,7 +30915,7 @@
     </row>
     <row r="216" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="70" t="s">
-        <v>772</v>
+        <v>782</v>
       </c>
       <c r="B216" s="48" t="s">
         <v>22</v>
@@ -30945,7 +30969,7 @@
         <v>22</v>
       </c>
       <c r="S216" s="49" t="s">
-        <v>859</v>
+        <v>842</v>
       </c>
       <c r="T216" s="48" t="s">
         <v>22</v>
@@ -30981,9 +31005,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="217" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="70" t="s">
-        <v>775</v>
+        <v>795</v>
       </c>
       <c r="B217" s="48" t="s">
         <v>22</v>
@@ -31037,7 +31061,7 @@
         <v>22</v>
       </c>
       <c r="S217" s="49" t="s">
-        <v>860</v>
+        <v>851</v>
       </c>
       <c r="T217" s="48" t="s">
         <v>22</v>
@@ -31066,16 +31090,16 @@
       <c r="AB217" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC217" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD217" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="218" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC217" s="82" t="s">
+        <v>877</v>
+      </c>
+      <c r="AD217" s="73" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="218" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="70" t="s">
-        <v>776</v>
+        <v>800</v>
       </c>
       <c r="B218" s="48" t="s">
         <v>22</v>
@@ -31129,7 +31153,7 @@
         <v>22</v>
       </c>
       <c r="S218" s="49" t="s">
-        <v>861</v>
+        <v>854</v>
       </c>
       <c r="T218" s="48" t="s">
         <v>22</v>
@@ -31158,16 +31182,16 @@
       <c r="AB218" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC218" s="48" t="s">
-        <v>22</v>
+      <c r="AC218" s="82" t="s">
+        <v>877</v>
       </c>
       <c r="AD218" s="48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="219" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="70" t="s">
-        <v>782</v>
+        <v>805</v>
       </c>
       <c r="B219" s="48" t="s">
         <v>22</v>
@@ -31221,10 +31245,10 @@
         <v>22</v>
       </c>
       <c r="S219" s="49" t="s">
-        <v>842</v>
-      </c>
-      <c r="T219" s="48" t="s">
-        <v>22</v>
+        <v>851</v>
+      </c>
+      <c r="T219" s="49" t="s">
+        <v>853</v>
       </c>
       <c r="U219" s="48" t="s">
         <v>22</v>
@@ -31250,16 +31274,16 @@
       <c r="AB219" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC219" s="48" t="s">
-        <v>22</v>
+      <c r="AC219" s="82" t="s">
+        <v>877</v>
       </c>
       <c r="AD219" s="48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="220" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:30" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="70" t="s">
-        <v>795</v>
+        <v>807</v>
       </c>
       <c r="B220" s="48" t="s">
         <v>22</v>
@@ -31315,8 +31339,8 @@
       <c r="S220" s="49" t="s">
         <v>851</v>
       </c>
-      <c r="T220" s="48" t="s">
-        <v>22</v>
+      <c r="T220" s="49" t="s">
+        <v>852</v>
       </c>
       <c r="U220" s="48" t="s">
         <v>22</v>
@@ -31345,13 +31369,13 @@
       <c r="AC220" s="82" t="s">
         <v>877</v>
       </c>
-      <c r="AD220" s="73" t="s">
-        <v>819</v>
+      <c r="AD220" s="48" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="221" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="70" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="B221" s="48" t="s">
         <v>22</v>
@@ -31405,7 +31429,7 @@
         <v>22</v>
       </c>
       <c r="S221" s="49" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="T221" s="48" t="s">
         <v>22</v>
@@ -31441,9 +31465,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="222" spans="1:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="70" t="s">
-        <v>805</v>
+        <v>814</v>
       </c>
       <c r="B222" s="48" t="s">
         <v>22</v>
@@ -31499,8 +31523,8 @@
       <c r="S222" s="49" t="s">
         <v>851</v>
       </c>
-      <c r="T222" s="49" t="s">
-        <v>853</v>
+      <c r="T222" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U222" s="48" t="s">
         <v>22</v>
@@ -31533,9 +31557,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="223" spans="1:30" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="70" t="s">
-        <v>807</v>
+        <v>816</v>
       </c>
       <c r="B223" s="48" t="s">
         <v>22</v>
@@ -31621,13 +31645,13 @@
       <c r="AC223" s="82" t="s">
         <v>877</v>
       </c>
-      <c r="AD223" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="224" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD223" s="73" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="224" spans="1:30" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="70" t="s">
-        <v>809</v>
+        <v>820</v>
       </c>
       <c r="B224" s="48" t="s">
         <v>22</v>
@@ -31683,8 +31707,8 @@
       <c r="S224" s="49" t="s">
         <v>851</v>
       </c>
-      <c r="T224" s="48" t="s">
-        <v>22</v>
+      <c r="T224" s="49" t="s">
+        <v>852</v>
       </c>
       <c r="U224" s="48" t="s">
         <v>22</v>
@@ -31719,7 +31743,7 @@
     </row>
     <row r="225" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="70" t="s">
-        <v>814</v>
+        <v>825</v>
       </c>
       <c r="B225" s="48" t="s">
         <v>22</v>
@@ -31809,9 +31833,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="226" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="70" t="s">
-        <v>816</v>
+        <v>828</v>
       </c>
       <c r="B226" s="48" t="s">
         <v>22</v>
@@ -31868,7 +31892,7 @@
         <v>851</v>
       </c>
       <c r="T226" s="49" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="U226" s="48" t="s">
         <v>22</v>
@@ -31897,13 +31921,13 @@
       <c r="AC226" s="82" t="s">
         <v>877</v>
       </c>
-      <c r="AD226" s="73" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="227" spans="1:30" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD226" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="227" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="70" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="B227" s="48" t="s">
         <v>22</v>
@@ -31960,7 +31984,7 @@
         <v>851</v>
       </c>
       <c r="T227" s="49" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="U227" s="48" t="s">
         <v>22</v>
@@ -31993,9 +32017,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="228" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="70" t="s">
-        <v>825</v>
+        <v>834</v>
       </c>
       <c r="B228" s="48" t="s">
         <v>22</v>
@@ -32051,8 +32075,8 @@
       <c r="S228" s="49" t="s">
         <v>851</v>
       </c>
-      <c r="T228" s="48" t="s">
-        <v>22</v>
+      <c r="T228" s="49" t="s">
+        <v>853</v>
       </c>
       <c r="U228" s="48" t="s">
         <v>22</v>
@@ -32085,9 +32109,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="229" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="70" t="s">
-        <v>828</v>
+        <v>862</v>
       </c>
       <c r="B229" s="48" t="s">
         <v>22</v>
@@ -32140,11 +32164,11 @@
       <c r="R229" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S229" s="49" t="s">
-        <v>851</v>
-      </c>
-      <c r="T229" s="49" t="s">
-        <v>853</v>
+      <c r="S229" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T229" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U229" s="48" t="s">
         <v>22</v>
@@ -32170,16 +32194,16 @@
       <c r="AB229" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC229" s="82" t="s">
-        <v>877</v>
+      <c r="AC229" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD229" s="48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="230" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="70" t="s">
-        <v>829</v>
+        <v>868</v>
       </c>
       <c r="B230" s="48" t="s">
         <v>22</v>
@@ -32232,11 +32256,11 @@
       <c r="R230" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S230" s="49" t="s">
-        <v>851</v>
-      </c>
-      <c r="T230" s="49" t="s">
-        <v>853</v>
+      <c r="S230" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T230" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U230" s="48" t="s">
         <v>22</v>
@@ -32262,8 +32286,8 @@
       <c r="AB230" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC230" s="82" t="s">
-        <v>877</v>
+      <c r="AC230" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD230" s="48" t="s">
         <v>22</v>
@@ -32271,7 +32295,7 @@
     </row>
     <row r="231" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="70" t="s">
-        <v>834</v>
+        <v>872</v>
       </c>
       <c r="B231" s="48" t="s">
         <v>22</v>
@@ -32324,11 +32348,11 @@
       <c r="R231" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S231" s="49" t="s">
-        <v>851</v>
-      </c>
-      <c r="T231" s="49" t="s">
-        <v>853</v>
+      <c r="S231" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T231" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U231" s="48" t="s">
         <v>22</v>
@@ -32354,8 +32378,8 @@
       <c r="AB231" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC231" s="82" t="s">
-        <v>877</v>
+      <c r="AC231" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD231" s="48" t="s">
         <v>22</v>
@@ -32363,7 +32387,7 @@
     </row>
     <row r="232" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="70" t="s">
-        <v>862</v>
+        <v>874</v>
       </c>
       <c r="B232" s="48" t="s">
         <v>22</v>
@@ -32446,8 +32470,8 @@
       <c r="AB232" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC232" s="48" t="s">
-        <v>22</v>
+      <c r="AC232" s="73" t="s">
+        <v>835</v>
       </c>
       <c r="AD232" s="48" t="s">
         <v>22</v>
@@ -32455,7 +32479,7 @@
     </row>
     <row r="233" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="70" t="s">
-        <v>868</v>
+        <v>888</v>
       </c>
       <c r="B233" s="48" t="s">
         <v>22</v>
@@ -32538,8 +32562,8 @@
       <c r="AB233" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC233" s="48" t="s">
-        <v>22</v>
+      <c r="AC233" s="73" t="s">
+        <v>889</v>
       </c>
       <c r="AD233" s="48" t="s">
         <v>22</v>
@@ -32547,7 +32571,7 @@
     </row>
     <row r="234" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="70" t="s">
-        <v>872</v>
+        <v>890</v>
       </c>
       <c r="B234" s="48" t="s">
         <v>22</v>
@@ -32630,286 +32654,10 @@
       <c r="AB234" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC234" s="48" t="s">
-        <v>22</v>
+      <c r="AC234" s="73" t="s">
+        <v>889</v>
       </c>
       <c r="AD234" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="235" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="70" t="s">
-        <v>874</v>
-      </c>
-      <c r="B235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="O235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="P235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="R235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="S235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="T235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="U235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="V235" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="W235" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X235" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA235" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB235" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC235" s="73" t="s">
-        <v>835</v>
-      </c>
-      <c r="AD235" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="236" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="70" t="s">
-        <v>888</v>
-      </c>
-      <c r="B236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="O236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="P236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="R236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="S236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="T236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="U236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="V236" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="W236" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X236" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA236" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB236" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC236" s="73" t="s">
-        <v>889</v>
-      </c>
-      <c r="AD236" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="237" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="70" t="s">
-        <v>890</v>
-      </c>
-      <c r="B237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="O237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="P237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="R237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="S237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="T237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="U237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="V237" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="W237" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X237" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA237" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB237" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC237" s="73" t="s">
-        <v>889</v>
-      </c>
-      <c r="AD237" s="48" t="s">
         <v>22</v>
       </c>
     </row>
@@ -33037,38 +32785,38 @@
     <hyperlink ref="G131" r:id="rId15" xr:uid="{27008350-2CEC-4E23-B4FE-4597862DB8D5}"/>
     <hyperlink ref="D142" r:id="rId16" xr:uid="{8898BD8E-2CA4-4CDE-890B-D65B515E0457}"/>
     <hyperlink ref="G172" r:id="rId17" xr:uid="{E0CF340A-567A-4979-87DE-4F467618A03F}"/>
-    <hyperlink ref="AC196" r:id="rId18" tooltip="Beige testing new" display="https://qa.zlta.testingserver8.com/product-detail/beige-testing-new" xr:uid="{2D91ED96-A11F-44E8-A3F9-04D2C908E6C3}"/>
-    <hyperlink ref="S186" r:id="rId19" display="https://opt.adm.testingserver8.com/admin/product-collection" xr:uid="{7E9C7A94-A136-40F4-8926-E175506C0FB0}"/>
-    <hyperlink ref="S200" r:id="rId20" xr:uid="{6E155B27-A1F3-4634-AF94-EA4AFCBB6FA8}"/>
-    <hyperlink ref="S178" r:id="rId21" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{FE84E4EC-8AD8-4353-9CF9-0FFD7AF22EC6}"/>
-    <hyperlink ref="S179" r:id="rId22" display="https://opt.adm.testingserver8.com/admin/home-page-banner" xr:uid="{FE688102-71E6-4D5D-8C26-E4A5C88965AB}"/>
-    <hyperlink ref="S180" r:id="rId23" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{75833417-6442-4309-8418-D565356A22B6}"/>
-    <hyperlink ref="S177" r:id="rId24" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{CF1B8F79-F4E1-4AB9-B852-9B1E92C5988C}"/>
-    <hyperlink ref="S181" r:id="rId25" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{B4C89834-3581-4298-A312-1087A98E46BC}"/>
-    <hyperlink ref="S182" r:id="rId26" display="https://opt.adm.testingserver8.com/admin/special-timer-event" xr:uid="{DC091BA2-1053-4AEE-9250-D6D43A208977}"/>
-    <hyperlink ref="S183" r:id="rId27" display="https://opt.adm.testingserver8.com/admin/categories" xr:uid="{6E9132F4-992B-46D1-9A28-5D473938DFF8}"/>
-    <hyperlink ref="S184" r:id="rId28" display="https://opt.adm.testingserver8.com/admin/product-collection" xr:uid="{B7714AD9-0B49-4F19-B276-CBDABCB03633}"/>
-    <hyperlink ref="S185" r:id="rId29" display="https://opt.adm.testingserver8.com/admin/categories" xr:uid="{965BF565-0242-4239-B278-6E574AF5D044}"/>
-    <hyperlink ref="S209" r:id="rId30" xr:uid="{C1127956-48DF-433C-AD28-9DA999FBCC26}"/>
-    <hyperlink ref="S208" r:id="rId31" xr:uid="{C9182A01-C96D-4110-9CA5-C017A54856E8}"/>
-    <hyperlink ref="S220" r:id="rId32" xr:uid="{6C20156C-B7E3-4D33-B99C-3A1821930139}"/>
-    <hyperlink ref="S225" r:id="rId33" xr:uid="{BAC34349-31E9-4520-A81D-6EEDD88BD29C}"/>
-    <hyperlink ref="S223" r:id="rId34" xr:uid="{95A32C29-884B-4748-92B0-EDDF6C5CE209}"/>
-    <hyperlink ref="S222" r:id="rId35" xr:uid="{118D0710-0BF2-49C8-888F-870ACC682CB5}"/>
-    <hyperlink ref="S226" r:id="rId36" xr:uid="{95BCE644-FF9B-472B-8145-F31A886E4FC4}"/>
-    <hyperlink ref="T226" r:id="rId37" xr:uid="{89BBFA7B-AD6E-4F93-BFD3-447AE8F7C502}"/>
-    <hyperlink ref="S227" r:id="rId38" xr:uid="{C8BD3F97-CFD5-4E09-8346-C525E3D0F983}"/>
-    <hyperlink ref="T227" r:id="rId39" display="https://console.zlaata.com/admin/return-order" xr:uid="{7EB489AF-7DBE-4776-BCF8-60461A79DB05}"/>
-    <hyperlink ref="S228" r:id="rId40" xr:uid="{570ACAD2-9993-464C-95C3-A0F384F535D4}"/>
-    <hyperlink ref="S229" r:id="rId41" xr:uid="{A5E4F190-F60E-4C69-A7BF-9E5AD6674C56}"/>
-    <hyperlink ref="S230" r:id="rId42" xr:uid="{0DD56580-2553-4B3D-AC00-0568BF6AD0B9}"/>
-    <hyperlink ref="S231" r:id="rId43" xr:uid="{16CBC571-4EE4-4D66-B8C3-CE0279FDD836}"/>
-    <hyperlink ref="T229" r:id="rId44" display="https://console.zlaata.com/admin/exchange-order" xr:uid="{5FB45239-0134-4C16-87DB-11C106356D92}"/>
-    <hyperlink ref="AD226" r:id="rId45" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{79B826CA-7F44-45A6-9BD2-CC8919CFA12A}"/>
-    <hyperlink ref="AC177" r:id="rId46" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{7BE8FE18-5C75-431B-8488-FBDEF16485E5}"/>
-    <hyperlink ref="AC178" r:id="rId47" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{FF640DAE-0F42-4B2A-A086-F1C73287AD75}"/>
-    <hyperlink ref="AC181" r:id="rId48" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{B625AA61-E1E0-4964-9CDD-901824C6555F}"/>
-    <hyperlink ref="AC235" r:id="rId49" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{622FD3BA-2464-4E1D-99AB-AE1AAC131875}"/>
+    <hyperlink ref="AC193" r:id="rId18" tooltip="Beige testing new" display="https://qa.zlta.testingserver8.com/product-detail/beige-testing-new" xr:uid="{2D91ED96-A11F-44E8-A3F9-04D2C908E6C3}"/>
+    <hyperlink ref="S183" r:id="rId19" display="https://opt.adm.testingserver8.com/admin/product-collection" xr:uid="{7E9C7A94-A136-40F4-8926-E175506C0FB0}"/>
+    <hyperlink ref="S197" r:id="rId20" xr:uid="{6E155B27-A1F3-4634-AF94-EA4AFCBB6FA8}"/>
+    <hyperlink ref="S175" r:id="rId21" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{FE84E4EC-8AD8-4353-9CF9-0FFD7AF22EC6}"/>
+    <hyperlink ref="S176" r:id="rId22" display="https://opt.adm.testingserver8.com/admin/home-page-banner" xr:uid="{FE688102-71E6-4D5D-8C26-E4A5C88965AB}"/>
+    <hyperlink ref="S177" r:id="rId23" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{75833417-6442-4309-8418-D565356A22B6}"/>
+    <hyperlink ref="S174" r:id="rId24" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{CF1B8F79-F4E1-4AB9-B852-9B1E92C5988C}"/>
+    <hyperlink ref="S178" r:id="rId25" display="https://opt.adm.testingserver8.com/admin/product" xr:uid="{B4C89834-3581-4298-A312-1087A98E46BC}"/>
+    <hyperlink ref="S179" r:id="rId26" display="https://opt.adm.testingserver8.com/admin/special-timer-event" xr:uid="{DC091BA2-1053-4AEE-9250-D6D43A208977}"/>
+    <hyperlink ref="S180" r:id="rId27" display="https://opt.adm.testingserver8.com/admin/categories" xr:uid="{6E9132F4-992B-46D1-9A28-5D473938DFF8}"/>
+    <hyperlink ref="S181" r:id="rId28" display="https://opt.adm.testingserver8.com/admin/product-collection" xr:uid="{B7714AD9-0B49-4F19-B276-CBDABCB03633}"/>
+    <hyperlink ref="S182" r:id="rId29" display="https://opt.adm.testingserver8.com/admin/categories" xr:uid="{965BF565-0242-4239-B278-6E574AF5D044}"/>
+    <hyperlink ref="S206" r:id="rId30" xr:uid="{C1127956-48DF-433C-AD28-9DA999FBCC26}"/>
+    <hyperlink ref="S205" r:id="rId31" xr:uid="{C9182A01-C96D-4110-9CA5-C017A54856E8}"/>
+    <hyperlink ref="S217" r:id="rId32" xr:uid="{6C20156C-B7E3-4D33-B99C-3A1821930139}"/>
+    <hyperlink ref="S222" r:id="rId33" xr:uid="{BAC34349-31E9-4520-A81D-6EEDD88BD29C}"/>
+    <hyperlink ref="S220" r:id="rId34" xr:uid="{95A32C29-884B-4748-92B0-EDDF6C5CE209}"/>
+    <hyperlink ref="S219" r:id="rId35" xr:uid="{118D0710-0BF2-49C8-888F-870ACC682CB5}"/>
+    <hyperlink ref="S223" r:id="rId36" xr:uid="{95BCE644-FF9B-472B-8145-F31A886E4FC4}"/>
+    <hyperlink ref="T223" r:id="rId37" xr:uid="{89BBFA7B-AD6E-4F93-BFD3-447AE8F7C502}"/>
+    <hyperlink ref="S224" r:id="rId38" xr:uid="{C8BD3F97-CFD5-4E09-8346-C525E3D0F983}"/>
+    <hyperlink ref="T224" r:id="rId39" display="https://console.zlaata.com/admin/return-order" xr:uid="{7EB489AF-7DBE-4776-BCF8-60461A79DB05}"/>
+    <hyperlink ref="S225" r:id="rId40" xr:uid="{570ACAD2-9993-464C-95C3-A0F384F535D4}"/>
+    <hyperlink ref="S226" r:id="rId41" xr:uid="{A5E4F190-F60E-4C69-A7BF-9E5AD6674C56}"/>
+    <hyperlink ref="S227" r:id="rId42" xr:uid="{0DD56580-2553-4B3D-AC00-0568BF6AD0B9}"/>
+    <hyperlink ref="S228" r:id="rId43" xr:uid="{16CBC571-4EE4-4D66-B8C3-CE0279FDD836}"/>
+    <hyperlink ref="T226" r:id="rId44" display="https://console.zlaata.com/admin/exchange-order" xr:uid="{5FB45239-0134-4C16-87DB-11C106356D92}"/>
+    <hyperlink ref="AD223" r:id="rId45" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{79B826CA-7F44-45A6-9BD2-CC8919CFA12A}"/>
+    <hyperlink ref="AC174" r:id="rId46" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{7BE8FE18-5C75-431B-8488-FBDEF16485E5}"/>
+    <hyperlink ref="AC175" r:id="rId47" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{FF640DAE-0F42-4B2A-A086-F1C73287AD75}"/>
+    <hyperlink ref="AC178" r:id="rId48" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{B625AA61-E1E0-4964-9CDD-901824C6555F}"/>
+    <hyperlink ref="AC232" r:id="rId49" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{622FD3BA-2464-4E1D-99AB-AE1AAC131875}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId50"/>
@@ -33079,7 +32827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67D78B6-EF58-4C2E-A040-EC8FC2ED5646}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New  test case inventories 2
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/zltUI/ZltTestData.xlsx
+++ b/src/test/resources/testdata/zltUI/ZltTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gowthamraj\git\ZlaataQAseverforme\src\test\resources\testdata\zltUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA66D8D0-37A9-4888-92FC-3249E80B8B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B099BEB5-A033-4FAD-BB3A-5ECBF8792E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-Zlaata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8446" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8524" uniqueCount="912">
   <si>
     <t>S.No</t>
   </si>
@@ -2744,6 +2744,24 @@
   </si>
   <si>
     <t>https://console.zlaata.com/admin/track-inventory</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_ADI_09</t>
+  </si>
+  <si>
+    <t>Verify that uploaded track inventory product count for two Product</t>
+  </si>
+  <si>
+    <t>TD_UI_Zlaata_ADI_09</t>
+  </si>
+  <si>
+    <t>TD_UI_Zlaata_ADI_10</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_ADI_10</t>
+  </si>
+  <si>
+    <t>Verify that the newly uploaded size in Track Inventory for a product is reflected in the application</t>
   </si>
 </sst>
 </file>
@@ -3380,24 +3398,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3424,6 +3424,24 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4227,10 +4245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75D1F84-2AD1-4552-9C1F-85B59D75CCFA}">
-  <dimension ref="A1:Z254"/>
+  <dimension ref="A1:Z256"/>
   <sheetViews>
-    <sheetView topLeftCell="D196" zoomScale="109" workbookViewId="0">
-      <selection activeCell="E214" sqref="E214"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4983,18 +5001,18 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="84" t="s">
+      <c r="A24" s="93" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="85"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
-      <c r="J24" s="86"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="95"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
@@ -5381,18 +5399,18 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="96" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="88"/>
-      <c r="C37" s="88"/>
-      <c r="D37" s="88"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="88"/>
-      <c r="G37" s="88"/>
-      <c r="H37" s="88"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="89"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="97"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="97"/>
+      <c r="H37" s="97"/>
+      <c r="I37" s="97"/>
+      <c r="J37" s="98"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
@@ -5939,18 +5957,18 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="87" t="s">
+      <c r="A55" s="96" t="s">
         <v>244</v>
       </c>
-      <c r="B55" s="88"/>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
-      <c r="E55" s="88"/>
-      <c r="F55" s="88"/>
-      <c r="G55" s="88"/>
-      <c r="H55" s="88"/>
-      <c r="I55" s="88"/>
-      <c r="J55" s="89"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="97"/>
+      <c r="D55" s="97"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+      <c r="I55" s="97"/>
+      <c r="J55" s="98"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="25">
@@ -6273,18 +6291,18 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="87" t="s">
+      <c r="A66" s="96" t="s">
         <v>246</v>
       </c>
-      <c r="B66" s="88"/>
-      <c r="C66" s="88"/>
-      <c r="D66" s="88"/>
-      <c r="E66" s="88"/>
-      <c r="F66" s="88"/>
-      <c r="G66" s="88"/>
-      <c r="H66" s="88"/>
-      <c r="I66" s="88"/>
-      <c r="J66" s="89"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="97"/>
+      <c r="D66" s="97"/>
+      <c r="E66" s="97"/>
+      <c r="F66" s="97"/>
+      <c r="G66" s="97"/>
+      <c r="H66" s="97"/>
+      <c r="I66" s="97"/>
+      <c r="J66" s="98"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="25">
@@ -6639,18 +6657,18 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="87" t="s">
+      <c r="A78" s="96" t="s">
         <v>345</v>
       </c>
-      <c r="B78" s="88"/>
-      <c r="C78" s="88"/>
-      <c r="D78" s="88"/>
-      <c r="E78" s="88"/>
-      <c r="F78" s="88"/>
-      <c r="G78" s="88"/>
-      <c r="H78" s="88"/>
-      <c r="I78" s="88"/>
-      <c r="J78" s="89"/>
+      <c r="B78" s="97"/>
+      <c r="C78" s="97"/>
+      <c r="D78" s="97"/>
+      <c r="E78" s="97"/>
+      <c r="F78" s="97"/>
+      <c r="G78" s="97"/>
+      <c r="H78" s="97"/>
+      <c r="I78" s="97"/>
+      <c r="J78" s="98"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="25">
@@ -7517,18 +7535,18 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="90" t="s">
+      <c r="A106" s="84" t="s">
         <v>374</v>
       </c>
-      <c r="B106" s="90"/>
-      <c r="C106" s="90"/>
-      <c r="D106" s="90"/>
-      <c r="E106" s="90"/>
-      <c r="F106" s="90"/>
-      <c r="G106" s="90"/>
-      <c r="H106" s="90"/>
-      <c r="I106" s="90"/>
-      <c r="J106" s="90"/>
+      <c r="B106" s="84"/>
+      <c r="C106" s="84"/>
+      <c r="D106" s="84"/>
+      <c r="E106" s="84"/>
+      <c r="F106" s="84"/>
+      <c r="G106" s="84"/>
+      <c r="H106" s="84"/>
+      <c r="I106" s="84"/>
+      <c r="J106" s="84"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="25">
@@ -8021,18 +8039,18 @@
       <c r="X120" s="58"/>
     </row>
     <row r="121" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="91" t="s">
+      <c r="A121" s="85" t="s">
         <v>376</v>
       </c>
-      <c r="B121" s="91"/>
-      <c r="C121" s="91"/>
-      <c r="D121" s="91"/>
-      <c r="E121" s="91"/>
-      <c r="F121" s="91"/>
-      <c r="G121" s="91"/>
-      <c r="H121" s="91"/>
-      <c r="I121" s="91"/>
-      <c r="J121" s="91"/>
+      <c r="B121" s="85"/>
+      <c r="C121" s="85"/>
+      <c r="D121" s="85"/>
+      <c r="E121" s="85"/>
+      <c r="F121" s="85"/>
+      <c r="G121" s="85"/>
+      <c r="H121" s="85"/>
+      <c r="I121" s="85"/>
+      <c r="J121" s="85"/>
       <c r="K121" s="57"/>
       <c r="L121" s="58"/>
       <c r="M121" s="58"/>
@@ -8095,18 +8113,18 @@
       <c r="X122" s="58"/>
     </row>
     <row r="123" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="91" t="s">
+      <c r="A123" s="85" t="s">
         <v>381</v>
       </c>
-      <c r="B123" s="91"/>
-      <c r="C123" s="91"/>
-      <c r="D123" s="91"/>
-      <c r="E123" s="91"/>
-      <c r="F123" s="91"/>
-      <c r="G123" s="91"/>
-      <c r="H123" s="91"/>
-      <c r="I123" s="91"/>
-      <c r="J123" s="91"/>
+      <c r="B123" s="85"/>
+      <c r="C123" s="85"/>
+      <c r="D123" s="85"/>
+      <c r="E123" s="85"/>
+      <c r="F123" s="85"/>
+      <c r="G123" s="85"/>
+      <c r="H123" s="85"/>
+      <c r="I123" s="85"/>
+      <c r="J123" s="85"/>
       <c r="K123" s="57"/>
       <c r="L123" s="58"/>
       <c r="M123" s="58"/>
@@ -8169,18 +8187,18 @@
       <c r="X124" s="58"/>
     </row>
     <row r="125" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="91" t="s">
+      <c r="A125" s="85" t="s">
         <v>394</v>
       </c>
-      <c r="B125" s="91"/>
-      <c r="C125" s="91"/>
-      <c r="D125" s="91"/>
-      <c r="E125" s="91"/>
-      <c r="F125" s="91"/>
-      <c r="G125" s="91"/>
-      <c r="H125" s="91"/>
-      <c r="I125" s="91"/>
-      <c r="J125" s="91"/>
+      <c r="B125" s="85"/>
+      <c r="C125" s="85"/>
+      <c r="D125" s="85"/>
+      <c r="E125" s="85"/>
+      <c r="F125" s="85"/>
+      <c r="G125" s="85"/>
+      <c r="H125" s="85"/>
+      <c r="I125" s="85"/>
+      <c r="J125" s="85"/>
     </row>
     <row r="126" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="25">
@@ -8505,18 +8523,18 @@
       <c r="X132" s="58"/>
     </row>
     <row r="133" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="91" t="s">
+      <c r="A133" s="85" t="s">
         <v>411</v>
       </c>
-      <c r="B133" s="91"/>
-      <c r="C133" s="91"/>
-      <c r="D133" s="92"/>
-      <c r="E133" s="92"/>
-      <c r="F133" s="92"/>
-      <c r="G133" s="92"/>
-      <c r="H133" s="92"/>
-      <c r="I133" s="92"/>
-      <c r="J133" s="92"/>
+      <c r="B133" s="85"/>
+      <c r="C133" s="85"/>
+      <c r="D133" s="86"/>
+      <c r="E133" s="86"/>
+      <c r="F133" s="86"/>
+      <c r="G133" s="86"/>
+      <c r="H133" s="86"/>
+      <c r="I133" s="86"/>
+      <c r="J133" s="86"/>
       <c r="K133" s="58"/>
       <c r="L133" s="58"/>
       <c r="M133" s="58"/>
@@ -9011,18 +9029,18 @@
       <c r="X144" s="58"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="96" t="s">
+      <c r="A145" s="90" t="s">
         <v>439</v>
       </c>
-      <c r="B145" s="97"/>
-      <c r="C145" s="97"/>
-      <c r="D145" s="97"/>
-      <c r="E145" s="97"/>
-      <c r="F145" s="97"/>
-      <c r="G145" s="97"/>
-      <c r="H145" s="97"/>
-      <c r="I145" s="97"/>
-      <c r="J145" s="98"/>
+      <c r="B145" s="91"/>
+      <c r="C145" s="91"/>
+      <c r="D145" s="91"/>
+      <c r="E145" s="91"/>
+      <c r="F145" s="91"/>
+      <c r="G145" s="91"/>
+      <c r="H145" s="91"/>
+      <c r="I145" s="91"/>
+      <c r="J145" s="92"/>
       <c r="K145" s="58"/>
       <c r="L145" s="58"/>
       <c r="M145" s="58"/>
@@ -9469,18 +9487,18 @@
       <c r="Z155" s="58"/>
     </row>
     <row r="156" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="91" t="s">
+      <c r="A156" s="85" t="s">
         <v>510</v>
       </c>
-      <c r="B156" s="91"/>
-      <c r="C156" s="91"/>
-      <c r="D156" s="91"/>
-      <c r="E156" s="91"/>
-      <c r="F156" s="91"/>
-      <c r="G156" s="91"/>
-      <c r="H156" s="91"/>
-      <c r="I156" s="91"/>
-      <c r="J156" s="91"/>
+      <c r="B156" s="85"/>
+      <c r="C156" s="85"/>
+      <c r="D156" s="85"/>
+      <c r="E156" s="85"/>
+      <c r="F156" s="85"/>
+      <c r="G156" s="85"/>
+      <c r="H156" s="85"/>
+      <c r="I156" s="85"/>
+      <c r="J156" s="85"/>
       <c r="K156" s="58"/>
       <c r="L156" s="58"/>
       <c r="M156" s="58"/>
@@ -9547,18 +9565,18 @@
       <c r="Z157" s="58"/>
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="91" t="s">
+      <c r="A158" s="85" t="s">
         <v>536</v>
       </c>
-      <c r="B158" s="91"/>
-      <c r="C158" s="91"/>
-      <c r="D158" s="91"/>
-      <c r="E158" s="91"/>
-      <c r="F158" s="91"/>
-      <c r="G158" s="91"/>
-      <c r="H158" s="91"/>
-      <c r="I158" s="91"/>
-      <c r="J158" s="91"/>
+      <c r="B158" s="85"/>
+      <c r="C158" s="85"/>
+      <c r="D158" s="85"/>
+      <c r="E158" s="85"/>
+      <c r="F158" s="85"/>
+      <c r="G158" s="85"/>
+      <c r="H158" s="85"/>
+      <c r="I158" s="85"/>
+      <c r="J158" s="85"/>
       <c r="K158" s="58"/>
       <c r="L158" s="58"/>
       <c r="M158" s="58"/>
@@ -10297,18 +10315,18 @@
       </c>
     </row>
     <row r="177" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="91" t="s">
+      <c r="A177" s="85" t="s">
         <v>715</v>
       </c>
-      <c r="B177" s="91"/>
-      <c r="C177" s="91"/>
+      <c r="B177" s="85"/>
+      <c r="C177" s="85"/>
       <c r="D177" s="83"/>
-      <c r="E177" s="91"/>
-      <c r="F177" s="91"/>
-      <c r="G177" s="91"/>
-      <c r="H177" s="91"/>
-      <c r="I177" s="91"/>
-      <c r="J177" s="91"/>
+      <c r="E177" s="85"/>
+      <c r="F177" s="85"/>
+      <c r="G177" s="85"/>
+      <c r="H177" s="85"/>
+      <c r="I177" s="85"/>
+      <c r="J177" s="85"/>
     </row>
     <row r="178" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="68">
@@ -10599,18 +10617,18 @@
       </c>
     </row>
     <row r="187" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="93" t="s">
+      <c r="A187" s="87" t="s">
         <v>617</v>
       </c>
-      <c r="B187" s="94"/>
-      <c r="C187" s="94"/>
-      <c r="D187" s="94"/>
-      <c r="E187" s="94"/>
-      <c r="F187" s="94"/>
-      <c r="G187" s="94"/>
-      <c r="H187" s="94"/>
-      <c r="I187" s="94"/>
-      <c r="J187" s="95"/>
+      <c r="B187" s="88"/>
+      <c r="C187" s="88"/>
+      <c r="D187" s="88"/>
+      <c r="E187" s="88"/>
+      <c r="F187" s="88"/>
+      <c r="G187" s="88"/>
+      <c r="H187" s="88"/>
+      <c r="I187" s="88"/>
+      <c r="J187" s="89"/>
     </row>
     <row r="188" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="68">
@@ -11295,43 +11313,61 @@
       </c>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A211" s="83" t="s">
-        <v>733</v>
-      </c>
-      <c r="B211" s="83"/>
-      <c r="C211" s="83"/>
-      <c r="D211" s="83"/>
-      <c r="E211" s="83"/>
-      <c r="F211" s="83"/>
-      <c r="G211" s="83"/>
-      <c r="H211" s="83"/>
-      <c r="I211" s="83"/>
-      <c r="J211" s="83"/>
+      <c r="A211" s="48">
+        <v>9</v>
+      </c>
+      <c r="B211" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C211" s="79" t="s">
+        <v>906</v>
+      </c>
+      <c r="D211" s="78" t="s">
+        <v>907</v>
+      </c>
+      <c r="E211" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F211" s="79" t="s">
+        <v>908</v>
+      </c>
+      <c r="G211" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H211" s="48" t="s">
+        <v>789</v>
+      </c>
+      <c r="I211" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J211" s="48" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="48">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B212" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C212" s="79" t="s">
-        <v>734</v>
+        <v>910</v>
       </c>
       <c r="D212" s="78" t="s">
-        <v>735</v>
+        <v>911</v>
       </c>
       <c r="E212" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F212" s="79" t="s">
-        <v>732</v>
+        <v>909</v>
       </c>
       <c r="G212" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H212" s="48" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="I212" s="48" t="s">
         <v>12</v>
@@ -11342,7 +11378,7 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="83" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B213" s="83"/>
       <c r="C213" s="83"/>
@@ -11362,22 +11398,22 @@
         <v>10</v>
       </c>
       <c r="C214" s="79" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="D214" s="78" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E214" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F214" s="79" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="G214" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H214" s="48" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="I214" s="48" t="s">
         <v>12</v>
@@ -11387,55 +11423,37 @@
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A215" s="48">
-        <v>2</v>
-      </c>
-      <c r="B215" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C215" s="79" t="s">
-        <v>741</v>
-      </c>
-      <c r="D215" s="78" t="s">
-        <v>742</v>
-      </c>
-      <c r="E215" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="F215" s="79" t="s">
-        <v>740</v>
-      </c>
-      <c r="G215" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="H215" s="48" t="s">
-        <v>791</v>
-      </c>
-      <c r="I215" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="J215" s="48" t="s">
-        <v>13</v>
-      </c>
+      <c r="A215" s="83" t="s">
+        <v>736</v>
+      </c>
+      <c r="B215" s="83"/>
+      <c r="C215" s="83"/>
+      <c r="D215" s="83"/>
+      <c r="E215" s="83"/>
+      <c r="F215" s="83"/>
+      <c r="G215" s="83"/>
+      <c r="H215" s="83"/>
+      <c r="I215" s="83"/>
+      <c r="J215" s="83"/>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B216" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C216" s="79" t="s">
-        <v>781</v>
+        <v>737</v>
       </c>
       <c r="D216" s="78" t="s">
-        <v>779</v>
+        <v>739</v>
       </c>
       <c r="E216" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F216" s="79" t="s">
-        <v>780</v>
+        <v>738</v>
       </c>
       <c r="G216" s="48" t="s">
         <v>11</v>
@@ -11452,22 +11470,22 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B217" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C217" s="79" t="s">
-        <v>868</v>
+        <v>741</v>
       </c>
       <c r="D217" s="78" t="s">
-        <v>869</v>
+        <v>742</v>
       </c>
       <c r="E217" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F217" s="79" t="s">
-        <v>870</v>
+        <v>740</v>
       </c>
       <c r="G217" s="48" t="s">
         <v>11</v>
@@ -11484,22 +11502,22 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B218" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C218" s="79" t="s">
-        <v>872</v>
+        <v>781</v>
       </c>
       <c r="D218" s="78" t="s">
-        <v>873</v>
+        <v>779</v>
       </c>
       <c r="E218" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F218" s="79" t="s">
-        <v>871</v>
+        <v>780</v>
       </c>
       <c r="G218" s="48" t="s">
         <v>11</v>
@@ -11515,43 +11533,61 @@
       </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A219" s="83" t="s">
-        <v>746</v>
-      </c>
-      <c r="B219" s="83"/>
-      <c r="C219" s="83"/>
-      <c r="D219" s="83"/>
-      <c r="E219" s="83"/>
-      <c r="F219" s="83"/>
-      <c r="G219" s="83"/>
-      <c r="H219" s="83"/>
-      <c r="I219" s="83"/>
-      <c r="J219" s="83"/>
+      <c r="A219" s="48">
+        <v>4</v>
+      </c>
+      <c r="B219" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C219" s="79" t="s">
+        <v>868</v>
+      </c>
+      <c r="D219" s="78" t="s">
+        <v>869</v>
+      </c>
+      <c r="E219" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F219" s="79" t="s">
+        <v>870</v>
+      </c>
+      <c r="G219" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H219" s="48" t="s">
+        <v>791</v>
+      </c>
+      <c r="I219" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J219" s="48" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="48">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B220" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C220" s="79" t="s">
-        <v>747</v>
+        <v>872</v>
       </c>
       <c r="D220" s="78" t="s">
-        <v>748</v>
+        <v>873</v>
       </c>
       <c r="E220" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F220" s="79" t="s">
-        <v>745</v>
+        <v>871</v>
       </c>
       <c r="G220" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H220" s="48" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="I220" s="48" t="s">
         <v>12</v>
@@ -11561,55 +11597,37 @@
       </c>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A221" s="48">
-        <v>2</v>
-      </c>
-      <c r="B221" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C221" s="79" t="s">
-        <v>749</v>
-      </c>
-      <c r="D221" s="78" t="s">
-        <v>750</v>
-      </c>
-      <c r="E221" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="F221" s="79" t="s">
-        <v>751</v>
-      </c>
-      <c r="G221" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="H221" s="48" t="s">
-        <v>792</v>
-      </c>
-      <c r="I221" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="J221" s="48" t="s">
-        <v>13</v>
-      </c>
+      <c r="A221" s="83" t="s">
+        <v>746</v>
+      </c>
+      <c r="B221" s="83"/>
+      <c r="C221" s="83"/>
+      <c r="D221" s="83"/>
+      <c r="E221" s="83"/>
+      <c r="F221" s="83"/>
+      <c r="G221" s="83"/>
+      <c r="H221" s="83"/>
+      <c r="I221" s="83"/>
+      <c r="J221" s="83"/>
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B222" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C222" s="79" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="D222" s="78" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="E222" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F222" s="79" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="G222" s="48" t="s">
         <v>11</v>
@@ -11626,22 +11644,22 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B223" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C223" s="79" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="D223" s="78" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="E223" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F223" s="79" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="G223" s="48" t="s">
         <v>11</v>
@@ -11658,22 +11676,22 @@
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B224" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C224" s="79" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="D224" s="78" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="E224" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F224" s="79" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="G224" s="48" t="s">
         <v>11</v>
@@ -11690,22 +11708,22 @@
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B225" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C225" s="79" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="D225" s="78" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="E225" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F225" s="79" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="G225" s="48" t="s">
         <v>11</v>
@@ -11722,22 +11740,22 @@
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="48">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B226" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C226" s="79" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="D226" s="78" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="E226" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F226" s="79" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="G226" s="48" t="s">
         <v>11</v>
@@ -11754,22 +11772,22 @@
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="48">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B227" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C227" s="79" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
       <c r="D227" s="78" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="E227" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F227" s="79" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="G227" s="48" t="s">
         <v>11</v>
@@ -11786,22 +11804,22 @@
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="48">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B228" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C228" s="79" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="D228" s="78" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="E228" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F228" s="79" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="G228" s="48" t="s">
         <v>11</v>
@@ -11818,22 +11836,22 @@
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="48">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B229" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C229" s="79" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="D229" s="78" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="E229" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F229" s="79" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="G229" s="48" t="s">
         <v>11</v>
@@ -11850,22 +11868,22 @@
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="48">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B230" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C230" s="79" t="s">
-        <v>777</v>
+        <v>770</v>
       </c>
       <c r="D230" s="78" t="s">
-        <v>778</v>
+        <v>771</v>
       </c>
       <c r="E230" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F230" s="79" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="G230" s="48" t="s">
         <v>11</v>
@@ -11880,44 +11898,62 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="83" t="s">
-        <v>783</v>
-      </c>
-      <c r="B231" s="83"/>
-      <c r="C231" s="83"/>
-      <c r="D231" s="83"/>
-      <c r="E231" s="83"/>
-      <c r="F231" s="83"/>
-      <c r="G231" s="83"/>
-      <c r="H231" s="83"/>
-      <c r="I231" s="83"/>
-      <c r="J231" s="83"/>
-    </row>
-    <row r="232" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231" s="48">
+        <v>10</v>
+      </c>
+      <c r="B231" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C231" s="79" t="s">
+        <v>773</v>
+      </c>
+      <c r="D231" s="78" t="s">
+        <v>774</v>
+      </c>
+      <c r="E231" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F231" s="79" t="s">
+        <v>775</v>
+      </c>
+      <c r="G231" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H231" s="48" t="s">
+        <v>792</v>
+      </c>
+      <c r="I231" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J231" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="48">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B232" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C232" s="79" t="s">
-        <v>794</v>
+        <v>777</v>
       </c>
       <c r="D232" s="78" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="E232" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F232" s="70" t="s">
-        <v>782</v>
+      <c r="F232" s="79" t="s">
+        <v>776</v>
       </c>
       <c r="G232" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H232" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="I232" s="48" t="s">
         <v>12</v>
@@ -11926,9 +11962,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="83" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="B233" s="83"/>
       <c r="C233" s="83"/>
@@ -11940,7 +11976,7 @@
       <c r="I233" s="83"/>
       <c r="J233" s="83"/>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="48">
         <v>1</v>
       </c>
@@ -11948,22 +11984,22 @@
         <v>10</v>
       </c>
       <c r="C234" s="79" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="D234" s="78" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="E234" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F234" s="79" t="s">
-        <v>795</v>
+      <c r="F234" s="70" t="s">
+        <v>782</v>
       </c>
       <c r="G234" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H234" s="48" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="I234" s="48" t="s">
         <v>12</v>
@@ -11973,55 +12009,37 @@
       </c>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A235" s="48">
-        <v>2</v>
-      </c>
-      <c r="B235" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C235" s="79" t="s">
-        <v>801</v>
-      </c>
-      <c r="D235" s="78" t="s">
-        <v>802</v>
-      </c>
-      <c r="E235" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="F235" s="79" t="s">
-        <v>800</v>
-      </c>
-      <c r="G235" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="H235" s="48" t="s">
-        <v>799</v>
-      </c>
-      <c r="I235" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="J235" s="48" t="s">
-        <v>13</v>
-      </c>
+      <c r="A235" s="83" t="s">
+        <v>796</v>
+      </c>
+      <c r="B235" s="83"/>
+      <c r="C235" s="83"/>
+      <c r="D235" s="83"/>
+      <c r="E235" s="83"/>
+      <c r="F235" s="83"/>
+      <c r="G235" s="83"/>
+      <c r="H235" s="83"/>
+      <c r="I235" s="83"/>
+      <c r="J235" s="83"/>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B236" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C236" s="79" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="D236" s="78" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="E236" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F236" s="79" t="s">
-        <v>805</v>
+        <v>795</v>
       </c>
       <c r="G236" s="48" t="s">
         <v>11</v>
@@ -12038,22 +12056,22 @@
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B237" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C237" s="79" t="s">
-        <v>808</v>
+        <v>801</v>
       </c>
       <c r="D237" s="78" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="E237" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F237" s="79" t="s">
-        <v>807</v>
+        <v>800</v>
       </c>
       <c r="G237" s="48" t="s">
         <v>11</v>
@@ -12070,22 +12088,22 @@
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B238" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C238" s="79" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="D238" s="78" t="s">
-        <v>811</v>
+        <v>804</v>
       </c>
       <c r="E238" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F238" s="79" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="G238" s="48" t="s">
         <v>11</v>
@@ -12102,22 +12120,22 @@
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B239" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C239" s="79" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D239" s="78" t="s">
-        <v>813</v>
+        <v>806</v>
       </c>
       <c r="E239" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F239" s="79" t="s">
-        <v>814</v>
+        <v>807</v>
       </c>
       <c r="G239" s="48" t="s">
         <v>11</v>
@@ -12134,22 +12152,22 @@
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="48">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B240" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C240" s="79" t="s">
-        <v>817</v>
+        <v>810</v>
       </c>
       <c r="D240" s="78" t="s">
-        <v>818</v>
+        <v>811</v>
       </c>
       <c r="E240" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F240" s="79" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
       <c r="G240" s="48" t="s">
         <v>11</v>
@@ -12166,22 +12184,22 @@
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="48">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B241" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C241" s="79" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="D241" s="78" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
       <c r="E241" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F241" s="79" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="G241" s="48" t="s">
         <v>11</v>
@@ -12198,22 +12216,22 @@
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="48">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B242" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C242" s="79" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="D242" s="78" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="E242" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F242" s="79" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
       <c r="G242" s="48" t="s">
         <v>11</v>
@@ -12230,22 +12248,22 @@
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="48">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B243" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C243" s="79" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="D243" s="78" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="E243" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F243" s="79" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="G243" s="48" t="s">
         <v>11</v>
@@ -12262,22 +12280,22 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="48">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B244" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C244" s="79" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="D244" s="78" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="E244" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F244" s="79" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="G244" s="48" t="s">
         <v>11</v>
@@ -12294,22 +12312,22 @@
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="48">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B245" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C245" s="79" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="D245" s="78" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="E245" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F245" s="79" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="G245" s="48" t="s">
         <v>11</v>
@@ -12324,44 +12342,62 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="83" t="s">
-        <v>841</v>
-      </c>
-      <c r="B246" s="83"/>
-      <c r="C246" s="83"/>
-      <c r="D246" s="83"/>
-      <c r="E246" s="83"/>
-      <c r="F246" s="83"/>
-      <c r="G246" s="83"/>
-      <c r="H246" s="83"/>
-      <c r="I246" s="83"/>
-      <c r="J246" s="83"/>
-    </row>
-    <row r="247" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A246" s="48">
+        <v>11</v>
+      </c>
+      <c r="B246" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C246" s="79" t="s">
+        <v>830</v>
+      </c>
+      <c r="D246" s="78" t="s">
+        <v>831</v>
+      </c>
+      <c r="E246" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F246" s="79" t="s">
+        <v>829</v>
+      </c>
+      <c r="G246" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H246" s="48" t="s">
+        <v>799</v>
+      </c>
+      <c r="I246" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J246" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="48">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B247" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C247" s="79" t="s">
-        <v>875</v>
+        <v>832</v>
       </c>
       <c r="D247" s="78" t="s">
-        <v>876</v>
+        <v>833</v>
       </c>
       <c r="E247" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F247" s="70" t="s">
-        <v>874</v>
+      <c r="F247" s="79" t="s">
+        <v>834</v>
       </c>
       <c r="G247" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H247" s="48" t="s">
-        <v>877</v>
+        <v>799</v>
       </c>
       <c r="I247" s="48" t="s">
         <v>12</v>
@@ -12371,75 +12407,75 @@
       </c>
     </row>
     <row r="248" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="48">
-        <v>2</v>
-      </c>
-      <c r="B248" s="48" t="s">
+      <c r="A248" s="83" t="s">
+        <v>841</v>
+      </c>
+      <c r="B248" s="83"/>
+      <c r="C248" s="83"/>
+      <c r="D248" s="83"/>
+      <c r="E248" s="83"/>
+      <c r="F248" s="83"/>
+      <c r="G248" s="83"/>
+      <c r="H248" s="83"/>
+      <c r="I248" s="83"/>
+      <c r="J248" s="83"/>
+    </row>
+    <row r="249" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="48">
+        <v>1</v>
+      </c>
+      <c r="B249" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C248" s="79" t="s">
-        <v>879</v>
-      </c>
-      <c r="D248" s="78" t="s">
-        <v>880</v>
-      </c>
-      <c r="E248" s="48" t="s">
+      <c r="C249" s="79" t="s">
+        <v>875</v>
+      </c>
+      <c r="D249" s="78" t="s">
+        <v>876</v>
+      </c>
+      <c r="E249" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F248" s="70" t="s">
-        <v>878</v>
-      </c>
-      <c r="G248" s="48" t="s">
+      <c r="F249" s="70" t="s">
+        <v>874</v>
+      </c>
+      <c r="G249" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="H248" s="48" t="s">
+      <c r="H249" s="48" t="s">
         <v>877</v>
       </c>
-      <c r="I248" s="48" t="s">
+      <c r="I249" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="J248" s="48" t="s">
+      <c r="J249" s="48" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="249" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="83" t="s">
-        <v>842</v>
-      </c>
-      <c r="B249" s="83"/>
-      <c r="C249" s="83"/>
-      <c r="D249" s="83"/>
-      <c r="E249" s="83"/>
-      <c r="F249" s="83"/>
-      <c r="G249" s="83"/>
-      <c r="H249" s="83"/>
-      <c r="I249" s="83"/>
-      <c r="J249" s="83"/>
     </row>
     <row r="250" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B250" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C250" s="79" t="s">
-        <v>843</v>
+        <v>879</v>
       </c>
       <c r="D250" s="78" t="s">
-        <v>846</v>
+        <v>880</v>
       </c>
       <c r="E250" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F250" s="70" t="s">
-        <v>844</v>
+        <v>878</v>
       </c>
       <c r="G250" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H250" s="48" t="s">
-        <v>845</v>
+        <v>877</v>
       </c>
       <c r="I250" s="48" t="s">
         <v>12</v>
@@ -12449,55 +12485,37 @@
       </c>
     </row>
     <row r="251" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="48">
-        <v>2</v>
-      </c>
-      <c r="B251" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C251" s="79" t="s">
-        <v>847</v>
-      </c>
-      <c r="D251" s="78" t="s">
-        <v>849</v>
-      </c>
-      <c r="E251" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="F251" s="70" t="s">
-        <v>848</v>
-      </c>
-      <c r="G251" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="H251" s="48" t="s">
-        <v>845</v>
-      </c>
-      <c r="I251" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="J251" s="48" t="s">
-        <v>13</v>
-      </c>
+      <c r="A251" s="83" t="s">
+        <v>842</v>
+      </c>
+      <c r="B251" s="83"/>
+      <c r="C251" s="83"/>
+      <c r="D251" s="83"/>
+      <c r="E251" s="83"/>
+      <c r="F251" s="83"/>
+      <c r="G251" s="83"/>
+      <c r="H251" s="83"/>
+      <c r="I251" s="83"/>
+      <c r="J251" s="83"/>
     </row>
     <row r="252" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B252" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C252" s="79" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="D252" s="78" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="E252" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F252" s="70" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="G252" s="48" t="s">
         <v>11</v>
@@ -12514,22 +12532,22 @@
     </row>
     <row r="253" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B253" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C253" s="79" t="s">
-        <v>861</v>
+        <v>847</v>
       </c>
       <c r="D253" s="78" t="s">
-        <v>862</v>
+        <v>849</v>
       </c>
       <c r="E253" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F253" s="70" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="G253" s="48" t="s">
         <v>11</v>
@@ -12546,22 +12564,22 @@
     </row>
     <row r="254" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B254" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C254" s="79" t="s">
-        <v>866</v>
+        <v>851</v>
       </c>
       <c r="D254" s="78" t="s">
-        <v>867</v>
+        <v>852</v>
       </c>
       <c r="E254" s="48" t="s">
         <v>14</v>
       </c>
       <c r="F254" s="70" t="s">
-        <v>865</v>
+        <v>850</v>
       </c>
       <c r="G254" s="48" t="s">
         <v>11</v>
@@ -12576,33 +12594,97 @@
         <v>13</v>
       </c>
     </row>
+    <row r="255" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="48">
+        <v>4</v>
+      </c>
+      <c r="B255" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C255" s="79" t="s">
+        <v>861</v>
+      </c>
+      <c r="D255" s="78" t="s">
+        <v>862</v>
+      </c>
+      <c r="E255" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F255" s="70" t="s">
+        <v>863</v>
+      </c>
+      <c r="G255" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H255" s="48" t="s">
+        <v>845</v>
+      </c>
+      <c r="I255" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J255" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="48">
+        <v>5</v>
+      </c>
+      <c r="B256" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C256" s="79" t="s">
+        <v>866</v>
+      </c>
+      <c r="D256" s="78" t="s">
+        <v>867</v>
+      </c>
+      <c r="E256" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F256" s="70" t="s">
+        <v>865</v>
+      </c>
+      <c r="G256" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H256" s="48" t="s">
+        <v>845</v>
+      </c>
+      <c r="I256" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J256" s="48" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A249:J249"/>
+    <mergeCell ref="A215:J215"/>
+    <mergeCell ref="A213:J213"/>
+    <mergeCell ref="A202:J202"/>
+    <mergeCell ref="A221:J221"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A55:J55"/>
+    <mergeCell ref="A66:J66"/>
+    <mergeCell ref="A78:J78"/>
+    <mergeCell ref="A251:J251"/>
     <mergeCell ref="A106:J106"/>
     <mergeCell ref="A121:J121"/>
     <mergeCell ref="A123:J123"/>
     <mergeCell ref="A125:J125"/>
     <mergeCell ref="A200:J200"/>
     <mergeCell ref="A195:J195"/>
-    <mergeCell ref="A246:J246"/>
-    <mergeCell ref="A233:J233"/>
+    <mergeCell ref="A248:J248"/>
+    <mergeCell ref="A235:J235"/>
     <mergeCell ref="A133:J133"/>
     <mergeCell ref="A187:J187"/>
     <mergeCell ref="A145:J145"/>
     <mergeCell ref="A156:J156"/>
     <mergeCell ref="A158:J158"/>
     <mergeCell ref="A177:J177"/>
-    <mergeCell ref="A231:J231"/>
-    <mergeCell ref="A213:J213"/>
-    <mergeCell ref="A211:J211"/>
-    <mergeCell ref="A202:J202"/>
-    <mergeCell ref="A219:J219"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="A55:J55"/>
-    <mergeCell ref="A66:J66"/>
-    <mergeCell ref="A78:J78"/>
+    <mergeCell ref="A233:J233"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="E2:J2 E8:J21 E23:J23">
@@ -12700,10 +12782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE74813B-34A6-48F5-8B35-1C10409ED694}">
-  <dimension ref="A1:AF239"/>
+  <dimension ref="A1:AF241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H193" workbookViewId="0">
-      <selection activeCell="S205" sqref="S205"/>
+    <sheetView topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="C202" sqref="C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29702,7 +29784,7 @@
     </row>
     <row r="203" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="70" t="s">
-        <v>732</v>
+        <v>908</v>
       </c>
       <c r="B203" s="48" t="s">
         <v>22</v>
@@ -29756,7 +29838,7 @@
         <v>22</v>
       </c>
       <c r="S203" s="49" t="s">
-        <v>882</v>
+        <v>905</v>
       </c>
       <c r="T203" s="48" t="s">
         <v>22</v>
@@ -29794,7 +29876,7 @@
     </row>
     <row r="204" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="70" t="s">
-        <v>738</v>
+        <v>909</v>
       </c>
       <c r="B204" s="48" t="s">
         <v>22</v>
@@ -29848,7 +29930,7 @@
         <v>22</v>
       </c>
       <c r="S204" s="49" t="s">
-        <v>890</v>
+        <v>905</v>
       </c>
       <c r="T204" s="48" t="s">
         <v>22</v>
@@ -29886,7 +29968,7 @@
     </row>
     <row r="205" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="70" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="B205" s="48" t="s">
         <v>22</v>
@@ -29940,7 +30022,7 @@
         <v>22</v>
       </c>
       <c r="S205" s="49" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="T205" s="48" t="s">
         <v>22</v>
@@ -29978,7 +30060,7 @@
     </row>
     <row r="206" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="70" t="s">
-        <v>780</v>
+        <v>738</v>
       </c>
       <c r="B206" s="48" t="s">
         <v>22</v>
@@ -30070,7 +30152,7 @@
     </row>
     <row r="207" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="70" t="s">
-        <v>870</v>
+        <v>740</v>
       </c>
       <c r="B207" s="48" t="s">
         <v>22</v>
@@ -30126,8 +30208,8 @@
       <c r="S207" s="49" t="s">
         <v>890</v>
       </c>
-      <c r="T207" s="49" t="s">
-        <v>891</v>
+      <c r="T207" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U207" s="48" t="s">
         <v>22</v>
@@ -30162,7 +30244,7 @@
     </row>
     <row r="208" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="70" t="s">
-        <v>871</v>
+        <v>780</v>
       </c>
       <c r="B208" s="48" t="s">
         <v>22</v>
@@ -30218,8 +30300,8 @@
       <c r="S208" s="49" t="s">
         <v>890</v>
       </c>
-      <c r="T208" s="49" t="s">
-        <v>891</v>
+      <c r="T208" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U208" s="48" t="s">
         <v>22</v>
@@ -30254,7 +30336,7 @@
     </row>
     <row r="209" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="70" t="s">
-        <v>745</v>
+        <v>870</v>
       </c>
       <c r="B209" s="48" t="s">
         <v>22</v>
@@ -30308,10 +30390,10 @@
         <v>22</v>
       </c>
       <c r="S209" s="49" t="s">
+        <v>890</v>
+      </c>
+      <c r="T209" s="49" t="s">
         <v>891</v>
-      </c>
-      <c r="T209" s="48" t="s">
-        <v>22</v>
       </c>
       <c r="U209" s="48" t="s">
         <v>22</v>
@@ -30346,7 +30428,7 @@
     </row>
     <row r="210" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="70" t="s">
-        <v>751</v>
+        <v>871</v>
       </c>
       <c r="B210" s="48" t="s">
         <v>22</v>
@@ -30400,10 +30482,10 @@
         <v>22</v>
       </c>
       <c r="S210" s="49" t="s">
-        <v>892</v>
-      </c>
-      <c r="T210" s="48" t="s">
-        <v>22</v>
+        <v>890</v>
+      </c>
+      <c r="T210" s="49" t="s">
+        <v>891</v>
       </c>
       <c r="U210" s="48" t="s">
         <v>22</v>
@@ -30438,7 +30520,7 @@
     </row>
     <row r="211" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="70" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="B211" s="48" t="s">
         <v>22</v>
@@ -30492,7 +30574,7 @@
         <v>22</v>
       </c>
       <c r="S211" s="49" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="T211" s="48" t="s">
         <v>22</v>
@@ -30530,7 +30612,7 @@
     </row>
     <row r="212" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="70" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="B212" s="48" t="s">
         <v>22</v>
@@ -30584,7 +30666,7 @@
         <v>22</v>
       </c>
       <c r="S212" s="49" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="T212" s="48" t="s">
         <v>22</v>
@@ -30622,7 +30704,7 @@
     </row>
     <row r="213" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="70" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="B213" s="48" t="s">
         <v>22</v>
@@ -30676,7 +30758,7 @@
         <v>22</v>
       </c>
       <c r="S213" s="49" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="T213" s="48" t="s">
         <v>22</v>
@@ -30714,7 +30796,7 @@
     </row>
     <row r="214" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="70" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B214" s="48" t="s">
         <v>22</v>
@@ -30768,7 +30850,7 @@
         <v>22</v>
       </c>
       <c r="S214" s="49" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="T214" s="48" t="s">
         <v>22</v>
@@ -30806,7 +30888,7 @@
     </row>
     <row r="215" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="70" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="B215" s="48" t="s">
         <v>22</v>
@@ -30860,7 +30942,7 @@
         <v>22</v>
       </c>
       <c r="S215" s="49" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="T215" s="48" t="s">
         <v>22</v>
@@ -30898,7 +30980,7 @@
     </row>
     <row r="216" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="70" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="B216" s="48" t="s">
         <v>22</v>
@@ -30952,7 +31034,7 @@
         <v>22</v>
       </c>
       <c r="S216" s="49" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="T216" s="48" t="s">
         <v>22</v>
@@ -30990,7 +31072,7 @@
     </row>
     <row r="217" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="70" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="B217" s="48" t="s">
         <v>22</v>
@@ -31044,7 +31126,7 @@
         <v>22</v>
       </c>
       <c r="S217" s="49" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="T217" s="48" t="s">
         <v>22</v>
@@ -31082,7 +31164,7 @@
     </row>
     <row r="218" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="70" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="B218" s="48" t="s">
         <v>22</v>
@@ -31136,7 +31218,7 @@
         <v>22</v>
       </c>
       <c r="S218" s="49" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="T218" s="48" t="s">
         <v>22</v>
@@ -31174,7 +31256,7 @@
     </row>
     <row r="219" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="70" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="B219" s="48" t="s">
         <v>22</v>
@@ -31228,7 +31310,7 @@
         <v>22</v>
       </c>
       <c r="S219" s="49" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="T219" s="48" t="s">
         <v>22</v>
@@ -31266,283 +31348,283 @@
     </row>
     <row r="220" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="70" t="s">
+        <v>775</v>
+      </c>
+      <c r="B220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S220" s="49" t="s">
+        <v>900</v>
+      </c>
+      <c r="T220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V220" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W220" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X220" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB220" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC220" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD220" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="221" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="70" t="s">
+        <v>776</v>
+      </c>
+      <c r="B221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S221" s="49" t="s">
+        <v>901</v>
+      </c>
+      <c r="T221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V221" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W221" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X221" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB221" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC221" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD221" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="222" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="70" t="s">
         <v>782</v>
       </c>
-      <c r="B220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="O220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="P220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="R220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="S220" s="49" t="s">
+      <c r="B222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S222" s="49" t="s">
         <v>882</v>
       </c>
-      <c r="T220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="U220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="V220" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="W220" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X220" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB220" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC220" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD220" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="221" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="70" t="s">
+      <c r="T222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V222" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W222" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X222" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB222" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC222" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD222" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="223" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="70" t="s">
         <v>795</v>
-      </c>
-      <c r="B221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="O221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="P221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="R221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="S221" s="49" t="s">
-        <v>891</v>
-      </c>
-      <c r="T221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="U221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="V221" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="W221" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X221" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA221" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB221" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC221" s="73" t="s">
-        <v>835</v>
-      </c>
-      <c r="AD221" s="73" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="222" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="70" t="s">
-        <v>800</v>
-      </c>
-      <c r="B222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="O222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="P222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="R222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="S222" s="49" t="s">
-        <v>894</v>
-      </c>
-      <c r="T222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="U222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="V222" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="W222" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X222" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA222" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB222" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC222" s="73" t="s">
-        <v>835</v>
-      </c>
-      <c r="AD222" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="223" spans="1:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="70" t="s">
-        <v>805</v>
       </c>
       <c r="B223" s="48" t="s">
         <v>22</v>
@@ -31598,8 +31680,8 @@
       <c r="S223" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="T223" s="49" t="s">
-        <v>893</v>
+      <c r="T223" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U223" s="48" t="s">
         <v>22</v>
@@ -31628,13 +31710,13 @@
       <c r="AC223" s="73" t="s">
         <v>835</v>
       </c>
-      <c r="AD223" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="224" spans="1:30" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD223" s="73" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="224" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="70" t="s">
-        <v>807</v>
+        <v>800</v>
       </c>
       <c r="B224" s="48" t="s">
         <v>22</v>
@@ -31688,10 +31770,10 @@
         <v>22</v>
       </c>
       <c r="S224" s="49" t="s">
-        <v>891</v>
-      </c>
-      <c r="T224" s="49" t="s">
-        <v>892</v>
+        <v>894</v>
+      </c>
+      <c r="T224" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U224" s="48" t="s">
         <v>22</v>
@@ -31724,9 +31806,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="225" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:30" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="70" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="B225" s="48" t="s">
         <v>22</v>
@@ -31782,8 +31864,8 @@
       <c r="S225" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="T225" s="48" t="s">
-        <v>22</v>
+      <c r="T225" s="49" t="s">
+        <v>893</v>
       </c>
       <c r="U225" s="48" t="s">
         <v>22</v>
@@ -31816,9 +31898,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="226" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:30" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="70" t="s">
-        <v>814</v>
+        <v>807</v>
       </c>
       <c r="B226" s="48" t="s">
         <v>22</v>
@@ -31874,8 +31956,8 @@
       <c r="S226" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="T226" s="48" t="s">
-        <v>22</v>
+      <c r="T226" s="49" t="s">
+        <v>892</v>
       </c>
       <c r="U226" s="48" t="s">
         <v>22</v>
@@ -31908,9 +31990,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="227" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="70" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
       <c r="B227" s="48" t="s">
         <v>22</v>
@@ -31966,8 +32048,8 @@
       <c r="S227" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="T227" s="49" t="s">
-        <v>892</v>
+      <c r="T227" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U227" s="48" t="s">
         <v>22</v>
@@ -31996,13 +32078,13 @@
       <c r="AC227" s="73" t="s">
         <v>835</v>
       </c>
-      <c r="AD227" s="73" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="228" spans="1:30" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD227" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="228" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="70" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="B228" s="48" t="s">
         <v>22</v>
@@ -32058,8 +32140,8 @@
       <c r="S228" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="T228" s="49" t="s">
-        <v>892</v>
+      <c r="T228" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U228" s="48" t="s">
         <v>22</v>
@@ -32092,9 +32174,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="229" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="70" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
       <c r="B229" s="48" t="s">
         <v>22</v>
@@ -32150,8 +32232,8 @@
       <c r="S229" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="T229" s="48" t="s">
-        <v>22</v>
+      <c r="T229" s="49" t="s">
+        <v>892</v>
       </c>
       <c r="U229" s="48" t="s">
         <v>22</v>
@@ -32180,13 +32262,13 @@
       <c r="AC229" s="73" t="s">
         <v>835</v>
       </c>
-      <c r="AD229" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="230" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD229" s="73" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="230" spans="1:30" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="70" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="B230" s="48" t="s">
         <v>22</v>
@@ -32243,7 +32325,7 @@
         <v>891</v>
       </c>
       <c r="T230" s="49" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="U230" s="48" t="s">
         <v>22</v>
@@ -32276,9 +32358,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="231" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="70" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="B231" s="48" t="s">
         <v>22</v>
@@ -32334,8 +32416,8 @@
       <c r="S231" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="T231" s="49" t="s">
-        <v>893</v>
+      <c r="T231" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="U231" s="48" t="s">
         <v>22</v>
@@ -32368,9 +32450,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="232" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="70" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="B232" s="48" t="s">
         <v>22</v>
@@ -32460,9 +32542,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="233" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:30" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="70" t="s">
-        <v>874</v>
+        <v>829</v>
       </c>
       <c r="B233" s="48" t="s">
         <v>22</v>
@@ -32515,11 +32597,11 @@
       <c r="R233" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S233" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="T233" s="48" t="s">
-        <v>22</v>
+      <c r="S233" s="49" t="s">
+        <v>891</v>
+      </c>
+      <c r="T233" s="49" t="s">
+        <v>893</v>
       </c>
       <c r="U233" s="48" t="s">
         <v>22</v>
@@ -32545,8 +32627,8 @@
       <c r="AB233" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC233" s="48" t="s">
-        <v>22</v>
+      <c r="AC233" s="73" t="s">
+        <v>835</v>
       </c>
       <c r="AD233" s="48" t="s">
         <v>22</v>
@@ -32554,7 +32636,7 @@
     </row>
     <row r="234" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="70" t="s">
-        <v>878</v>
+        <v>834</v>
       </c>
       <c r="B234" s="48" t="s">
         <v>22</v>
@@ -32607,11 +32689,11 @@
       <c r="R234" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="S234" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="T234" s="48" t="s">
-        <v>22</v>
+      <c r="S234" s="49" t="s">
+        <v>891</v>
+      </c>
+      <c r="T234" s="49" t="s">
+        <v>893</v>
       </c>
       <c r="U234" s="48" t="s">
         <v>22</v>
@@ -32637,8 +32719,8 @@
       <c r="AB234" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC234" s="48" t="s">
-        <v>22</v>
+      <c r="AC234" s="73" t="s">
+        <v>835</v>
       </c>
       <c r="AD234" s="48" t="s">
         <v>22</v>
@@ -32646,7 +32728,7 @@
     </row>
     <row r="235" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="70" t="s">
-        <v>844</v>
+        <v>874</v>
       </c>
       <c r="B235" s="48" t="s">
         <v>22</v>
@@ -32738,7 +32820,7 @@
     </row>
     <row r="236" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="70" t="s">
-        <v>848</v>
+        <v>878</v>
       </c>
       <c r="B236" s="48" t="s">
         <v>22</v>
@@ -32830,7 +32912,7 @@
     </row>
     <row r="237" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="70" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="B237" s="48" t="s">
         <v>22</v>
@@ -32913,8 +32995,8 @@
       <c r="AB237" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC237" s="73" t="s">
-        <v>835</v>
+      <c r="AC237" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD237" s="48" t="s">
         <v>22</v>
@@ -32922,7 +33004,7 @@
     </row>
     <row r="238" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="70" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="B238" s="48" t="s">
         <v>22</v>
@@ -33005,8 +33087,8 @@
       <c r="AB238" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AC238" s="73" t="s">
-        <v>864</v>
+      <c r="AC238" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="AD238" s="48" t="s">
         <v>22</v>
@@ -33014,93 +33096,277 @@
     </row>
     <row r="239" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="70" t="s">
+        <v>850</v>
+      </c>
+      <c r="B239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V239" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W239" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X239" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA239" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB239" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC239" s="73" t="s">
+        <v>835</v>
+      </c>
+      <c r="AD239" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="240" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="70" t="s">
+        <v>863</v>
+      </c>
+      <c r="B240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V240" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W240" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X240" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA240" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB240" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC240" s="73" t="s">
+        <v>864</v>
+      </c>
+      <c r="AD240" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="241" spans="1:30" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="70" t="s">
         <v>865</v>
       </c>
-      <c r="B239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="G239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="H239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="J239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="K239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="L239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="M239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="N239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="O239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="P239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="R239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="S239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="T239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="U239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="V239" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="W239" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="X239" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA239" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB239" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC239" s="73" t="s">
+      <c r="B241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V241" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W241" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X241" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA241" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB241" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC241" s="73" t="s">
         <v>864</v>
       </c>
-      <c r="AD239" s="48" t="s">
+      <c r="AD241" s="48" t="s">
         <v>22</v>
       </c>
     </row>
@@ -33240,35 +33506,37 @@
     <hyperlink ref="S181" r:id="rId27" display="https://opt.adm.testingserver8.com/admin/categories" xr:uid="{6E9132F4-992B-46D1-9A28-5D473938DFF8}"/>
     <hyperlink ref="S182" r:id="rId28" display="https://opt.adm.testingserver8.com/admin/product-collection" xr:uid="{B7714AD9-0B49-4F19-B276-CBDABCB03633}"/>
     <hyperlink ref="S183" r:id="rId29" display="https://opt.adm.testingserver8.com/admin/categories" xr:uid="{965BF565-0242-4239-B278-6E574AF5D044}"/>
-    <hyperlink ref="S210" r:id="rId30" display="https://qa.adm.testingserver8.com/admin/return-order" xr:uid="{C1127956-48DF-433C-AD28-9DA999FBCC26}"/>
-    <hyperlink ref="S209" r:id="rId31" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{C9182A01-C96D-4110-9CA5-C017A54856E8}"/>
-    <hyperlink ref="S221" r:id="rId32" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{6C20156C-B7E3-4D33-B99C-3A1821930139}"/>
-    <hyperlink ref="S226" r:id="rId33" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{BAC34349-31E9-4520-A81D-6EEDD88BD29C}"/>
-    <hyperlink ref="S224" r:id="rId34" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{95A32C29-884B-4748-92B0-EDDF6C5CE209}"/>
-    <hyperlink ref="S223" r:id="rId35" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{118D0710-0BF2-49C8-888F-870ACC682CB5}"/>
-    <hyperlink ref="S227" r:id="rId36" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{95BCE644-FF9B-472B-8145-F31A886E4FC4}"/>
-    <hyperlink ref="T227" r:id="rId37" display="https://qa.adm.testingserver8.com/admin/return-order" xr:uid="{89BBFA7B-AD6E-4F93-BFD3-447AE8F7C502}"/>
-    <hyperlink ref="S228" r:id="rId38" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{C8BD3F97-CFD5-4E09-8346-C525E3D0F983}"/>
-    <hyperlink ref="T228" r:id="rId39" xr:uid="{7EB489AF-7DBE-4776-BCF8-60461A79DB05}"/>
-    <hyperlink ref="S229" r:id="rId40" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{570ACAD2-9993-464C-95C3-A0F384F535D4}"/>
-    <hyperlink ref="S230" r:id="rId41" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{A5E4F190-F60E-4C69-A7BF-9E5AD6674C56}"/>
-    <hyperlink ref="S231" r:id="rId42" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{0DD56580-2553-4B3D-AC00-0568BF6AD0B9}"/>
-    <hyperlink ref="S232" r:id="rId43" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{16CBC571-4EE4-4D66-B8C3-CE0279FDD836}"/>
-    <hyperlink ref="T230" r:id="rId44" xr:uid="{5FB45239-0134-4C16-87DB-11C106356D92}"/>
-    <hyperlink ref="AD227" r:id="rId45" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{79B826CA-7F44-45A6-9BD2-CC8919CFA12A}"/>
+    <hyperlink ref="S212" r:id="rId30" display="https://qa.adm.testingserver8.com/admin/return-order" xr:uid="{C1127956-48DF-433C-AD28-9DA999FBCC26}"/>
+    <hyperlink ref="S211" r:id="rId31" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{C9182A01-C96D-4110-9CA5-C017A54856E8}"/>
+    <hyperlink ref="S223" r:id="rId32" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{6C20156C-B7E3-4D33-B99C-3A1821930139}"/>
+    <hyperlink ref="S228" r:id="rId33" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{BAC34349-31E9-4520-A81D-6EEDD88BD29C}"/>
+    <hyperlink ref="S226" r:id="rId34" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{95A32C29-884B-4748-92B0-EDDF6C5CE209}"/>
+    <hyperlink ref="S225" r:id="rId35" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{118D0710-0BF2-49C8-888F-870ACC682CB5}"/>
+    <hyperlink ref="S229" r:id="rId36" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{95BCE644-FF9B-472B-8145-F31A886E4FC4}"/>
+    <hyperlink ref="T229" r:id="rId37" display="https://qa.adm.testingserver8.com/admin/return-order" xr:uid="{89BBFA7B-AD6E-4F93-BFD3-447AE8F7C502}"/>
+    <hyperlink ref="S230" r:id="rId38" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{C8BD3F97-CFD5-4E09-8346-C525E3D0F983}"/>
+    <hyperlink ref="T230" r:id="rId39" xr:uid="{7EB489AF-7DBE-4776-BCF8-60461A79DB05}"/>
+    <hyperlink ref="S231" r:id="rId40" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{570ACAD2-9993-464C-95C3-A0F384F535D4}"/>
+    <hyperlink ref="S232" r:id="rId41" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{A5E4F190-F60E-4C69-A7BF-9E5AD6674C56}"/>
+    <hyperlink ref="S233" r:id="rId42" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{0DD56580-2553-4B3D-AC00-0568BF6AD0B9}"/>
+    <hyperlink ref="S234" r:id="rId43" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{16CBC571-4EE4-4D66-B8C3-CE0279FDD836}"/>
+    <hyperlink ref="T232" r:id="rId44" xr:uid="{5FB45239-0134-4C16-87DB-11C106356D92}"/>
+    <hyperlink ref="AD229" r:id="rId45" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{79B826CA-7F44-45A6-9BD2-CC8919CFA12A}"/>
     <hyperlink ref="AC175" r:id="rId46" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{7BE8FE18-5C75-431B-8488-FBDEF16485E5}"/>
     <hyperlink ref="AC176" r:id="rId47" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{FF640DAE-0F42-4B2A-A086-F1C73287AD75}"/>
     <hyperlink ref="AC179" r:id="rId48" tooltip="Blue dskjjksdjkdjds" display="https://qa.zlta.testingserver8.com/product-detail/blue-dskjjksdjkdjds" xr:uid="{B625AA61-E1E0-4964-9CDD-901824C6555F}"/>
-    <hyperlink ref="AC237" r:id="rId49" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{622FD3BA-2464-4E1D-99AB-AE1AAC131875}"/>
-    <hyperlink ref="T207" r:id="rId50" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{7F5A23D3-57AD-40E6-ACE3-9B9EA550F6A6}"/>
-    <hyperlink ref="T208" r:id="rId51" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{7C8D8F70-AFD1-452B-AFB6-66EC6F975597}"/>
+    <hyperlink ref="AC239" r:id="rId49" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{622FD3BA-2464-4E1D-99AB-AE1AAC131875}"/>
+    <hyperlink ref="T209" r:id="rId50" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{7F5A23D3-57AD-40E6-ACE3-9B9EA550F6A6}"/>
+    <hyperlink ref="T210" r:id="rId51" display="https://qa.adm.testingserver8.com/admin/order" xr:uid="{7C8D8F70-AFD1-452B-AFB6-66EC6F975597}"/>
     <hyperlink ref="S197" r:id="rId52" display="https://qa.adm.testingserver8.com/admin/product-style" xr:uid="{279698D4-2A41-4BBD-838A-CBE141EE3D50}"/>
-    <hyperlink ref="AC221" r:id="rId53" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{CD96CCCF-BE60-40A1-BA2F-93729430B99A}"/>
-    <hyperlink ref="AC222:AC232" r:id="rId54" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{C68B94AD-4CFE-4AB2-9431-B829C1D5A48C}"/>
-    <hyperlink ref="S215" r:id="rId55" display="https://qa.zlta.testingserver8.com/admin/payment-pending" xr:uid="{37E5E50E-434D-4FC0-B9A6-C0648E88FF97}"/>
-    <hyperlink ref="S202" r:id="rId56" xr:uid="{C356118E-7CF8-4DBB-80E8-2AC4DA83F153}"/>
+    <hyperlink ref="AC223" r:id="rId53" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{CD96CCCF-BE60-40A1-BA2F-93729430B99A}"/>
+    <hyperlink ref="AC224:AC234" r:id="rId54" tooltip="Crop Waistcoat Set" display="https://testing.zlaata.com/product-detail/purple-ikat-waistcoat-pant-cotton-co-ord-set" xr:uid="{C68B94AD-4CFE-4AB2-9431-B829C1D5A48C}"/>
+    <hyperlink ref="S217" r:id="rId55" display="https://qa.zlta.testingserver8.com/admin/payment-pending" xr:uid="{37E5E50E-434D-4FC0-B9A6-C0648E88FF97}"/>
+    <hyperlink ref="S204" r:id="rId56" xr:uid="{C356118E-7CF8-4DBB-80E8-2AC4DA83F153}"/>
+    <hyperlink ref="S202" r:id="rId57" xr:uid="{51EDB8E8-7B87-48E3-AE6E-CF4598B89047}"/>
+    <hyperlink ref="S203" r:id="rId58" xr:uid="{F9518A74-6EB1-4B3C-A794-D43A85FC89FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId57"/>
+  <pageSetup orientation="portrait" r:id="rId59"/>
 </worksheet>
 </file>
</xml_diff>